<commit_message>
added common method for search
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12405" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4935" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Y</t>
   </si>
@@ -97,6 +97,33 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Battaramulla</t>
+  </si>
+  <si>
+    <t>Kandy</t>
+  </si>
+  <si>
+    <t>Kalutara</t>
+  </si>
+  <si>
+    <t>Jaela</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>loc1</t>
+  </si>
+  <si>
+    <t>loc2</t>
+  </si>
+  <si>
+    <t>loc3</t>
+  </si>
+  <si>
+    <t>loc4</t>
   </si>
 </sst>
 </file>
@@ -425,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +485,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,6 +513,62 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fine tuned search column/rows and verifying results. added common methods
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4935" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13830" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L17"/>
+  <oleSize ref="A1:K17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -114,16 +114,16 @@
     <t>Inactive</t>
   </si>
   <si>
-    <t>loc1</t>
-  </si>
-  <si>
-    <t>loc2</t>
-  </si>
-  <si>
-    <t>loc3</t>
-  </si>
-  <si>
-    <t>loc4</t>
+    <t>loc13</t>
+  </si>
+  <si>
+    <t>loc23d</t>
+  </si>
+  <si>
+    <t>loc33d</t>
+  </si>
+  <si>
+    <t>loc43e</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modifed click method to include javascirpt click; code refactoring for row verification
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13830" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -114,16 +114,16 @@
     <t>Inactive</t>
   </si>
   <si>
-    <t>loc13</t>
-  </si>
-  <si>
-    <t>loc23d</t>
-  </si>
-  <si>
-    <t>loc33d</t>
-  </si>
-  <si>
-    <t>loc43e</t>
+    <t>nn01</t>
+  </si>
+  <si>
+    <t>nn02</t>
+  </si>
+  <si>
+    <t>abc00</t>
+  </si>
+  <si>
+    <t>uuy</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added more images and speciefied path to testcase from excel; added + button click on insttitue add; refactored verifyrecordsave method
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K17"/>
+  <oleSize ref="A1:M17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Y</t>
   </si>
@@ -114,16 +114,37 @@
     <t>Inactive</t>
   </si>
   <si>
-    <t>nn01</t>
-  </si>
-  <si>
-    <t>nn02</t>
-  </si>
-  <si>
-    <t>abc00</t>
-  </si>
-  <si>
-    <t>uuy</t>
+    <t>+94777998990</t>
+  </si>
+  <si>
+    <t>+94777654321</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>src/test/resources/images/logo.jpg</t>
+  </si>
+  <si>
+    <t>src/test/resources/images/img1.jpg</t>
+  </si>
+  <si>
+    <t>src/test/resources/images/img2.jpg</t>
+  </si>
+  <si>
+    <t>+94666543345</t>
+  </si>
+  <si>
+    <t>branch1</t>
+  </si>
+  <si>
+    <t>bra2</t>
+  </si>
+  <si>
+    <t>brrr3</t>
+  </si>
+  <si>
+    <t>b333</t>
   </si>
 </sst>
 </file>
@@ -168,9 +189,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -518,7 +540,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -532,7 +554,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -546,7 +568,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -560,7 +582,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
@@ -584,15 +606,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -603,13 +630,16 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -619,14 +649,17 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>2222</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -636,14 +669,17 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>3333</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -653,10 +689,13 @@
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
-        <v>3333</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -667,6 +706,7 @@
     <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added check for uploading non-image file as logo for institute
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M17"/>
+  <oleSize ref="A1:J17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Y</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>b333</t>
+  </si>
+  <si>
+    <t>yyy@yyy.lk</t>
+  </si>
+  <si>
+    <t>ACBT</t>
+  </si>
+  <si>
+    <t>src/test/resources/images/Audit_Feedback.rtf</t>
   </si>
 </sst>
 </file>
@@ -476,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -606,16 +615,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -690,12 +699,32 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -704,9 +733,10 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added common method to set status; added test for adding new centers
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\eclipse-workspace\SLIIT_Automation\src\test\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
     <sheet name="add_institute_details" sheetId="8" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId3"/>
+    <sheet name="add_new_centers" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>Y</t>
   </si>
@@ -78,15 +82,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>loc001</t>
-  </si>
-  <si>
-    <t>loc002</t>
-  </si>
-  <si>
-    <t>loc003</t>
-  </si>
-  <si>
     <t>Colombo</t>
   </si>
   <si>
@@ -135,18 +130,6 @@
     <t>+94666543345</t>
   </si>
   <si>
-    <t>branch1</t>
-  </si>
-  <si>
-    <t>bra2</t>
-  </si>
-  <si>
-    <t>brrr3</t>
-  </si>
-  <si>
-    <t>b333</t>
-  </si>
-  <si>
     <t>yyy@yyy.lk</t>
   </si>
   <si>
@@ -154,6 +137,78 @@
   </si>
   <si>
     <t>src/test/resources/images/Audit_Feedback.rtf</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>exam center</t>
+  </si>
+  <si>
+    <t>library</t>
+  </si>
+  <si>
+    <t>canteen</t>
+  </si>
+  <si>
+    <t>recreation area</t>
+  </si>
+  <si>
+    <t>wash room</t>
+  </si>
+  <si>
+    <t>malabe</t>
+  </si>
+  <si>
+    <t>colombo</t>
+  </si>
+  <si>
+    <t>metro</t>
+  </si>
+  <si>
+    <t>jaela</t>
+  </si>
+  <si>
+    <t>kandy</t>
+  </si>
+  <si>
+    <t>CENx</t>
+  </si>
+  <si>
+    <t>CENy</t>
+  </si>
+  <si>
+    <t>CENi</t>
+  </si>
+  <si>
+    <t>CEN1</t>
+  </si>
+  <si>
+    <t>CEN-</t>
+  </si>
+  <si>
+    <t>CEN00</t>
+  </si>
+  <si>
+    <t>loc999</t>
+  </si>
+  <si>
+    <t>loczbc</t>
+  </si>
+  <si>
+    <t>locdfdfdf</t>
+  </si>
+  <si>
+    <t>loc093</t>
+  </si>
+  <si>
+    <t>loc34343</t>
+  </si>
+  <si>
+    <t>loc---</t>
+  </si>
+  <si>
+    <t>locxxxx</t>
   </si>
 </sst>
 </file>
@@ -483,15 +538,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -505,99 +560,99 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C8" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -617,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -639,7 +694,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -659,10 +714,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -679,10 +734,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -699,10 +754,10 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -710,19 +765,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -742,12 +797,134 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added center search method; modified center adding test case to include avilable locations
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>Y</t>
   </si>
@@ -157,39 +157,6 @@
     <t>wash room</t>
   </si>
   <si>
-    <t>malabe</t>
-  </si>
-  <si>
-    <t>colombo</t>
-  </si>
-  <si>
-    <t>metro</t>
-  </si>
-  <si>
-    <t>jaela</t>
-  </si>
-  <si>
-    <t>kandy</t>
-  </si>
-  <si>
-    <t>CENx</t>
-  </si>
-  <si>
-    <t>CENy</t>
-  </si>
-  <si>
-    <t>CENi</t>
-  </si>
-  <si>
-    <t>CEN1</t>
-  </si>
-  <si>
-    <t>CEN-</t>
-  </si>
-  <si>
-    <t>CEN00</t>
-  </si>
-  <si>
     <t>loc999</t>
   </si>
   <si>
@@ -209,13 +176,40 @@
   </si>
   <si>
     <t>locxxxx</t>
+  </si>
+  <si>
+    <t>ordercheck</t>
+  </si>
+  <si>
+    <t>Inactive location</t>
+  </si>
+  <si>
+    <t>NEW 11</t>
+  </si>
+  <si>
+    <t>CEN90</t>
+  </si>
+  <si>
+    <t>CEN91</t>
+  </si>
+  <si>
+    <t>CEN92</t>
+  </si>
+  <si>
+    <t>CEN93</t>
+  </si>
+  <si>
+    <t>CEN94</t>
+  </si>
+  <si>
+    <t>CEN95</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +224,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF565656"/>
+      <name val="Metropolis"/>
     </font>
   </fonts>
   <fills count="2">
@@ -253,10 +252,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -540,13 +540,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -560,9 +560,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -574,9 +574,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -588,9 +588,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -602,9 +602,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -616,9 +616,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -630,9 +630,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -644,9 +644,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -676,14 +676,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -703,7 +703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -763,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -799,13 +799,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -822,15 +822,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>44</v>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -839,15 +839,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
-        <v>45</v>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -856,15 +856,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -873,15 +873,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
-        <v>46</v>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -890,15 +890,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -907,15 +907,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
-        <v>43</v>
+      <c r="C7" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
added center search and center edit tests; modified verify row values method to elminiate x mark
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
     <sheet name="add_institute_details" sheetId="8" r:id="rId2"/>
     <sheet name="add_new_centers" sheetId="7" r:id="rId3"/>
+    <sheet name="view_centers" sheetId="10" r:id="rId4"/>
+    <sheet name="edit_centers" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="74">
   <si>
     <t>Y</t>
   </si>
@@ -203,6 +205,51 @@
   </si>
   <si>
     <t>CEN95</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>new code</t>
+  </si>
+  <si>
+    <t>new name</t>
+  </si>
+  <si>
+    <t>MCEN1</t>
+  </si>
+  <si>
+    <t>MCEN2</t>
+  </si>
+  <si>
+    <t>MCEN3</t>
+  </si>
+  <si>
+    <t>MCEN4</t>
+  </si>
+  <si>
+    <t>NewName1</t>
+  </si>
+  <si>
+    <t>NewName2</t>
+  </si>
+  <si>
+    <t>NewName3</t>
+  </si>
+  <si>
+    <t>NewName4</t>
   </si>
 </sst>
 </file>
@@ -799,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -927,4 +974,151 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added method to verify table records show in descending order
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="view_centers" sheetId="10" r:id="rId4"/>
     <sheet name="edit_centers" sheetId="11" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
   <si>
     <t>Y</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Head office</t>
   </si>
   <si>
-    <t>sliit@sltnet.lk</t>
-  </si>
-  <si>
     <t>NIBM</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>Kandy</t>
   </si>
   <si>
-    <t>Kalutara</t>
-  </si>
-  <si>
     <t>Jaela</t>
   </si>
   <si>
@@ -159,54 +153,6 @@
     <t>wash room</t>
   </si>
   <si>
-    <t>loc999</t>
-  </si>
-  <si>
-    <t>loczbc</t>
-  </si>
-  <si>
-    <t>locdfdfdf</t>
-  </si>
-  <si>
-    <t>loc093</t>
-  </si>
-  <si>
-    <t>loc34343</t>
-  </si>
-  <si>
-    <t>loc---</t>
-  </si>
-  <si>
-    <t>locxxxx</t>
-  </si>
-  <si>
-    <t>ordercheck</t>
-  </si>
-  <si>
-    <t>Inactive location</t>
-  </si>
-  <si>
-    <t>NEW 11</t>
-  </si>
-  <si>
-    <t>CEN90</t>
-  </si>
-  <si>
-    <t>CEN91</t>
-  </si>
-  <si>
-    <t>CEN92</t>
-  </si>
-  <si>
-    <t>CEN93</t>
-  </si>
-  <si>
-    <t>CEN94</t>
-  </si>
-  <si>
-    <t>CEN95</t>
-  </si>
-  <si>
     <t>row</t>
   </si>
   <si>
@@ -250,13 +196,58 @@
   </si>
   <si>
     <t>NewName4</t>
+  </si>
+  <si>
+    <t>Kalutara2</t>
+  </si>
+  <si>
+    <t>sliit@slt.net</t>
+  </si>
+  <si>
+    <t>LOC456</t>
+  </si>
+  <si>
+    <t>LOC457</t>
+  </si>
+  <si>
+    <t>LOC458</t>
+  </si>
+  <si>
+    <t>LOC459</t>
+  </si>
+  <si>
+    <t>LOC460</t>
+  </si>
+  <si>
+    <t>LOC461</t>
+  </si>
+  <si>
+    <t>LOC462</t>
+  </si>
+  <si>
+    <t>CENTER789</t>
+  </si>
+  <si>
+    <t>CENTER790</t>
+  </si>
+  <si>
+    <t>CENTER791</t>
+  </si>
+  <si>
+    <t>CENTER792</t>
+  </si>
+  <si>
+    <t>CENTER793</t>
+  </si>
+  <si>
+    <t>CENTER794</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,11 +262,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF565656"/>
-      <name val="Metropolis"/>
     </font>
   </fonts>
   <fills count="2">
@@ -299,11 +285,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -588,118 +573,118 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -720,17 +705,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -741,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -750,7 +735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -758,73 +743,73 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -846,126 +831,129 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
@@ -981,49 +969,49 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -1039,80 +1027,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
added new test case for adding departments
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="add_new_centers" sheetId="7" r:id="rId3"/>
     <sheet name="view_centers" sheetId="10" r:id="rId4"/>
     <sheet name="edit_centers" sheetId="11" r:id="rId5"/>
+    <sheet name="add_new_departments" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
   <si>
     <t>Y</t>
   </si>
@@ -241,6 +242,48 @@
   </si>
   <si>
     <t>CENTER794</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>faculty</t>
+  </si>
+  <si>
+    <t>Exmaination</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Graphics</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Sarath</t>
+  </si>
+  <si>
+    <t>Mahin</t>
+  </si>
+  <si>
+    <t>DEPT008</t>
+  </si>
+  <si>
+    <t>DEPT009</t>
+  </si>
+  <si>
+    <t>DEPT010</t>
+  </si>
+  <si>
+    <t>DEPT011</t>
+  </si>
+  <si>
+    <t>DEPT012</t>
   </si>
 </sst>
 </file>
@@ -831,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1109,4 +1152,139 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed data set included all tests in the testngxml
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -175,18 +175,6 @@
     <t>new name</t>
   </si>
   <si>
-    <t>MCEN1</t>
-  </si>
-  <si>
-    <t>MCEN2</t>
-  </si>
-  <si>
-    <t>MCEN3</t>
-  </si>
-  <si>
-    <t>MCEN4</t>
-  </si>
-  <si>
     <t>NewName1</t>
   </si>
   <si>
@@ -205,45 +193,6 @@
     <t>sliit@slt.net</t>
   </si>
   <si>
-    <t>LOC456</t>
-  </si>
-  <si>
-    <t>LOC457</t>
-  </si>
-  <si>
-    <t>LOC458</t>
-  </si>
-  <si>
-    <t>LOC459</t>
-  </si>
-  <si>
-    <t>LOC460</t>
-  </si>
-  <si>
-    <t>LOC461</t>
-  </si>
-  <si>
-    <t>LOC462</t>
-  </si>
-  <si>
-    <t>CENTER789</t>
-  </si>
-  <si>
-    <t>CENTER790</t>
-  </si>
-  <si>
-    <t>CENTER791</t>
-  </si>
-  <si>
-    <t>CENTER792</t>
-  </si>
-  <si>
-    <t>CENTER793</t>
-  </si>
-  <si>
-    <t>CENTER794</t>
-  </si>
-  <si>
     <t>head</t>
   </si>
   <si>
@@ -271,19 +220,70 @@
     <t>Mahin</t>
   </si>
   <si>
-    <t>DEPT008</t>
-  </si>
-  <si>
-    <t>DEPT009</t>
-  </si>
-  <si>
-    <t>DEPT010</t>
-  </si>
-  <si>
-    <t>DEPT011</t>
-  </si>
-  <si>
-    <t>DEPT012</t>
+    <t>DEPT0081</t>
+  </si>
+  <si>
+    <t>DEPT0082</t>
+  </si>
+  <si>
+    <t>DEPT0083</t>
+  </si>
+  <si>
+    <t>DEPT0084</t>
+  </si>
+  <si>
+    <t>DEPT0085</t>
+  </si>
+  <si>
+    <t>MCEN13</t>
+  </si>
+  <si>
+    <t>MCEN14</t>
+  </si>
+  <si>
+    <t>MCEN15</t>
+  </si>
+  <si>
+    <t>MCEN16</t>
+  </si>
+  <si>
+    <t>CENTER7891</t>
+  </si>
+  <si>
+    <t>CENTER7892</t>
+  </si>
+  <si>
+    <t>CENTER7893</t>
+  </si>
+  <si>
+    <t>CENTER7894</t>
+  </si>
+  <si>
+    <t>CENTER7895</t>
+  </si>
+  <si>
+    <t>CENTER7896</t>
+  </si>
+  <si>
+    <t>LOC777</t>
+  </si>
+  <si>
+    <t>LOC778</t>
+  </si>
+  <si>
+    <t>LOC779</t>
+  </si>
+  <si>
+    <t>LOC780</t>
+  </si>
+  <si>
+    <t>LOC781</t>
+  </si>
+  <si>
+    <t>LOC782</t>
+  </si>
+  <si>
+    <t>LOC783</t>
   </si>
 </sst>
 </file>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +637,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -707,10 +707,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -786,7 +786,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>28</v>
@@ -875,7 +875,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +902,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -936,7 +936,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -987,7 +987,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -1071,7 +1071,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,10 +1098,10 @@
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1112,10 +1112,10 @@
         <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1126,10 +1126,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1140,10 +1140,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1158,7 +1158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
@@ -1172,10 +1172,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -1186,16 +1186,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -1206,16 +1206,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -1226,16 +1226,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -1246,16 +1246,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1266,16 +1266,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
added tests for dept search / view / edit
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="view_centers" sheetId="10" r:id="rId4"/>
     <sheet name="edit_centers" sheetId="11" r:id="rId5"/>
     <sheet name="add_new_departments" sheetId="12" r:id="rId6"/>
+    <sheet name="view_departments" sheetId="13" r:id="rId7"/>
+    <sheet name="edit_departments" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="93">
   <si>
     <t>Y</t>
   </si>
@@ -284,6 +286,30 @@
   </si>
   <si>
     <t>LOC783</t>
+  </si>
+  <si>
+    <t>DEPT_updated_0081</t>
+  </si>
+  <si>
+    <t>DEPT_updated_0082</t>
+  </si>
+  <si>
+    <t>DEPT_updated_0083</t>
+  </si>
+  <si>
+    <t>DEPT_updated_0084</t>
+  </si>
+  <si>
+    <t>Dept_name_udpated_99</t>
+  </si>
+  <si>
+    <t>Dept_name_udpated_100</t>
+  </si>
+  <si>
+    <t>Dept_name_udpated_101</t>
+  </si>
+  <si>
+    <t>Dept_name_udpated_102</t>
   </si>
 </sst>
 </file>
@@ -615,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1287,4 +1313,151 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed prefix by adding Auto_ for codes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -177,18 +177,6 @@
     <t>new name</t>
   </si>
   <si>
-    <t>NewName1</t>
-  </si>
-  <si>
-    <t>NewName2</t>
-  </si>
-  <si>
-    <t>NewName3</t>
-  </si>
-  <si>
-    <t>NewName4</t>
-  </si>
-  <si>
     <t>Kalutara2</t>
   </si>
   <si>
@@ -222,94 +210,106 @@
     <t>Mahin</t>
   </si>
   <si>
-    <t>DEPT0081</t>
-  </si>
-  <si>
-    <t>DEPT0082</t>
-  </si>
-  <si>
-    <t>DEPT0083</t>
-  </si>
-  <si>
-    <t>DEPT0084</t>
-  </si>
-  <si>
-    <t>DEPT0085</t>
-  </si>
-  <si>
-    <t>MCEN13</t>
-  </si>
-  <si>
-    <t>MCEN14</t>
-  </si>
-  <si>
-    <t>MCEN15</t>
-  </si>
-  <si>
-    <t>MCEN16</t>
-  </si>
-  <si>
-    <t>CENTER7891</t>
-  </si>
-  <si>
-    <t>CENTER7892</t>
-  </si>
-  <si>
-    <t>CENTER7893</t>
-  </si>
-  <si>
-    <t>CENTER7894</t>
-  </si>
-  <si>
-    <t>CENTER7895</t>
-  </si>
-  <si>
-    <t>CENTER7896</t>
-  </si>
-  <si>
-    <t>LOC777</t>
-  </si>
-  <si>
-    <t>LOC778</t>
-  </si>
-  <si>
-    <t>LOC779</t>
-  </si>
-  <si>
-    <t>LOC780</t>
-  </si>
-  <si>
-    <t>LOC781</t>
-  </si>
-  <si>
-    <t>LOC782</t>
-  </si>
-  <si>
-    <t>LOC783</t>
-  </si>
-  <si>
-    <t>DEPT_updated_0081</t>
-  </si>
-  <si>
-    <t>DEPT_updated_0082</t>
-  </si>
-  <si>
-    <t>DEPT_updated_0083</t>
-  </si>
-  <si>
-    <t>DEPT_updated_0084</t>
-  </si>
-  <si>
-    <t>Dept_name_udpated_99</t>
-  </si>
-  <si>
-    <t>Dept_name_udpated_100</t>
-  </si>
-  <si>
-    <t>Dept_name_udpated_101</t>
-  </si>
-  <si>
-    <t>Dept_name_udpated_102</t>
+    <t>Auto_LOC27771</t>
+  </si>
+  <si>
+    <t>Auto_LOC27772</t>
+  </si>
+  <si>
+    <t>Auto_LOC27773</t>
+  </si>
+  <si>
+    <t>Auto_LOC27774</t>
+  </si>
+  <si>
+    <t>Auto_LOC27775</t>
+  </si>
+  <si>
+    <t>Auto_LOC27776</t>
+  </si>
+  <si>
+    <t>Auto_LOC27777</t>
+  </si>
+  <si>
+    <t>Auto_CENTER1987</t>
+  </si>
+  <si>
+    <t>Auto_CENTER1988</t>
+  </si>
+  <si>
+    <t>Auto_CENTER1989</t>
+  </si>
+  <si>
+    <t>Auto_CENTER1990</t>
+  </si>
+  <si>
+    <t>Auto_CENTER1991</t>
+  </si>
+  <si>
+    <t>Auto_CENTER1992</t>
+  </si>
+  <si>
+    <t>Auto_UPDATED_CEN113</t>
+  </si>
+  <si>
+    <t>Auto_UPDATED_CEN114</t>
+  </si>
+  <si>
+    <t>Auto_UPDATED_CEN115</t>
+  </si>
+  <si>
+    <t>Auto_UPDATED_CEN116</t>
+  </si>
+  <si>
+    <t>Auto_DEPT00811</t>
+  </si>
+  <si>
+    <t>Auto_DEPT00812</t>
+  </si>
+  <si>
+    <t>Auto_DEPT00813</t>
+  </si>
+  <si>
+    <t>Auto_DEPT00814</t>
+  </si>
+  <si>
+    <t>Auto_DEPT00815</t>
+  </si>
+  <si>
+    <t>Auto_DEPT_updated_0181</t>
+  </si>
+  <si>
+    <t>Auto_DEPT_updated_0182</t>
+  </si>
+  <si>
+    <t>Auto_DEPT_updated_0183</t>
+  </si>
+  <si>
+    <t>Auto_DEPT_updated_0184</t>
+  </si>
+  <si>
+    <t>Auto_Dept_name_udpated_99</t>
+  </si>
+  <si>
+    <t>Auto_Dept_name_udpated_100</t>
+  </si>
+  <si>
+    <t>Auto_Dept_name_udpated_101</t>
+  </si>
+  <si>
+    <t>Auto_Dept_name_udpated_102</t>
+  </si>
+  <si>
+    <t>Auto_UPDATED_CENTER_X765</t>
+  </si>
+  <si>
+    <t>Auto_UPDATED_CENTER_X766</t>
+  </si>
+  <si>
+    <t>Auto_UPDATED_CENTER_X767</t>
+  </si>
+  <si>
+    <t>Auto_UPDATED_CENTER_X768</t>
   </si>
 </sst>
 </file>
@@ -642,7 +642,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +663,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -733,10 +733,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +812,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>28</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -1097,7 +1097,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,10 +1124,10 @@
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1138,10 +1138,10 @@
         <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1152,10 +1152,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1166,10 +1166,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1185,7 +1185,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,10 +1198,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -1212,16 +1212,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -1232,16 +1232,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -1252,16 +1252,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -1272,16 +1272,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1292,16 +1292,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -1378,13 +1378,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,10 +1407,10 @@
         <v>42</v>
       </c>
       <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1420,10 +1421,10 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1434,10 +1435,10 @@
         <v>44</v>
       </c>
       <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1448,10 +1449,10 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
added tests for faculty. added common method to retrive active column values
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="add_new_departments" sheetId="12" r:id="rId6"/>
     <sheet name="view_departments" sheetId="13" r:id="rId7"/>
     <sheet name="edit_departments" sheetId="14" r:id="rId8"/>
+    <sheet name="add_new_faculty" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="106">
   <si>
     <t>Y</t>
   </si>
@@ -310,6 +311,45 @@
   </si>
   <si>
     <t>Auto_Dept_name_102</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>Auto_FCT001</t>
+  </si>
+  <si>
+    <t>Auto_FCT002</t>
+  </si>
+  <si>
+    <t>Auto_FCT003</t>
+  </si>
+  <si>
+    <t>Auto_FCT004</t>
+  </si>
+  <si>
+    <t>Auto_FCT005</t>
+  </si>
+  <si>
+    <t>Auto_FCT006</t>
+  </si>
+  <si>
+    <t>abcdefghi jklimnop 123</t>
+  </si>
+  <si>
+    <t>abcdefghi jklimnop 124</t>
+  </si>
+  <si>
+    <t>abcdefghi jklimnop 125</t>
+  </si>
+  <si>
+    <t>abcdefghi jklimnop 126</t>
+  </si>
+  <si>
+    <t>abcdefghi jklimnop 127</t>
+  </si>
+  <si>
+    <t>abcdefghi jklimnop 128</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
@@ -1461,4 +1501,124 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified awarding institute search method to read data from excel; fixed institute adding test case where remove telephone numbers was not handled before
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="view_departments" sheetId="13" r:id="rId7"/>
     <sheet name="edit_departments" sheetId="14" r:id="rId8"/>
     <sheet name="add_new_faculty" sheetId="15" r:id="rId9"/>
+    <sheet name="add_new_awarding_institute" sheetId="16" r:id="rId10"/>
+    <sheet name="view_awarding_institutes" sheetId="17" r:id="rId11"/>
+    <sheet name="search_awarding_institute" sheetId="19" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="120">
   <si>
     <t>Y</t>
   </si>
@@ -109,12 +112,6 @@
     <t>Inactive</t>
   </si>
   <si>
-    <t>+94777998990</t>
-  </si>
-  <si>
-    <t>+94777654321</t>
-  </si>
-  <si>
     <t>logo</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>src/test/resources/images/img2.jpg</t>
   </si>
   <si>
-    <t>+94666543345</t>
-  </si>
-  <si>
     <t>yyy@yyy.lk</t>
   </si>
   <si>
@@ -350,6 +344,57 @@
   </si>
   <si>
     <t>abcdefghi jklimnop 128</t>
+  </si>
+  <si>
+    <t>Auto_AI001</t>
+  </si>
+  <si>
+    <t>Auto_AI002</t>
+  </si>
+  <si>
+    <t>Auto_AI003</t>
+  </si>
+  <si>
+    <t>Auto_AI004</t>
+  </si>
+  <si>
+    <t>Auto_AI005</t>
+  </si>
+  <si>
+    <t>Curtin</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>Hallam</t>
+  </si>
+  <si>
+    <t>UGC</t>
+  </si>
+  <si>
+    <t>EDU</t>
+  </si>
+  <si>
+    <t>+94777222222</t>
+  </si>
+  <si>
+    <t>+94777653333</t>
+  </si>
+  <si>
+    <t>+94666544444</t>
+  </si>
+  <si>
+    <t>+94666545555</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>inactive</t>
   </si>
 </sst>
 </file>
@@ -703,7 +748,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -717,7 +762,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -731,7 +776,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -745,7 +790,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -759,7 +804,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -773,10 +818,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -787,7 +832,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -809,19 +854,235 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="5" max="5" width="25.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -835,7 +1096,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -852,13 +1113,13 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -875,10 +1136,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -895,10 +1156,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -906,19 +1167,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -957,7 +1218,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -968,10 +1229,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -985,10 +1246,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -1002,10 +1263,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -1019,10 +1280,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -1036,10 +1297,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -1053,10 +1314,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -1088,7 +1349,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1096,7 +1357,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1104,7 +1365,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1112,7 +1373,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1120,7 +1381,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -1147,13 +1408,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1161,13 +1422,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1175,13 +1436,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1189,13 +1450,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1203,13 +1464,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1238,10 +1499,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -1252,16 +1513,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -1272,16 +1533,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -1292,16 +1553,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -1312,16 +1573,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
         <v>55</v>
       </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1332,16 +1593,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -1370,7 +1631,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1378,7 +1639,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1386,7 +1647,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1394,7 +1655,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1402,7 +1663,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -1430,13 +1691,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1444,13 +1705,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1458,13 +1719,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1472,13 +1733,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1486,13 +1747,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1507,7 +1768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
@@ -1525,7 +1786,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1536,10 +1797,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -1550,10 +1811,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -1564,10 +1825,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -1578,10 +1839,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -1592,10 +1853,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
@@ -1606,10 +1867,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
edit awarding institute & Xpaths for classrooms and doc types
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20348"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\eclipse-workspace\SLIIT_Automation\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF4DB0B-4A42-494A-97AF-3F8912FAD5EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -24,8 +25,17 @@
     <sheet name="add_new_awarding_institute" sheetId="16" r:id="rId10"/>
     <sheet name="view_awarding_institutes" sheetId="17" r:id="rId11"/>
     <sheet name="search_awarding_institute" sheetId="19" r:id="rId12"/>
+    <sheet name="edit_awarding_institute" sheetId="20" r:id="rId13"/>
+    <sheet name="add_new_classrooms" sheetId="21" r:id="rId14"/>
+    <sheet name="search_classrooms" sheetId="22" r:id="rId15"/>
+    <sheet name="view_classrooms" sheetId="28" r:id="rId16"/>
+    <sheet name="edit_classrooms" sheetId="29" r:id="rId17"/>
+    <sheet name="add_new_document_type" sheetId="23" r:id="rId18"/>
+    <sheet name="view_document_type" sheetId="25" r:id="rId19"/>
+    <sheet name="search_document_type" sheetId="24" r:id="rId20"/>
+    <sheet name="edit_document_type" sheetId="27" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="141">
   <si>
     <t>Y</t>
   </si>
@@ -395,12 +405,75 @@
   </si>
   <si>
     <t>inactive</t>
+  </si>
+  <si>
+    <t>Auto_AI_upd_0100</t>
+  </si>
+  <si>
+    <t>Auto_AI_upd_0101</t>
+  </si>
+  <si>
+    <t>Auto_AI_upd_0102</t>
+  </si>
+  <si>
+    <t>Auto_AI_upd_0103</t>
+  </si>
+  <si>
+    <t>Auto_AI_name_99</t>
+  </si>
+  <si>
+    <t>Auto_AI_name_100</t>
+  </si>
+  <si>
+    <t>Auto_AI_name_101</t>
+  </si>
+  <si>
+    <t>Auto_AI_name_102</t>
+  </si>
+  <si>
+    <t>D-Block 301</t>
+  </si>
+  <si>
+    <t>study capacity</t>
+  </si>
+  <si>
+    <t>exam capacity</t>
+  </si>
+  <si>
+    <t>Auto_CR_R-001</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Birth Certificate</t>
+  </si>
+  <si>
+    <t>Auto_DT_001</t>
+  </si>
+  <si>
+    <t>Birth</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Auto_DT_upd_0100</t>
+  </si>
+  <si>
+    <t>Auto_DT_name_99</t>
+  </si>
+  <si>
+    <t>Auto_CR_upd_0100</t>
+  </si>
+  <si>
+    <t>Auto_CR_name_99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,10 +512,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -723,7 +797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -846,20 +920,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="sliit@sltnet.lk"/>
-    <hyperlink ref="C3" r:id="rId2" display="nibm@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="idm@idm.net"/>
+    <hyperlink ref="C2" r:id="rId1" display="sliit@sltnet.lk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" display="nibm@gmail.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display="idm@idm.net" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,11 +1031,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,11 +1090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,8 +1144,346 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44361976-27BE-4654-ADCA-E167640F93C3}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66064CB0-35F9-4B0A-8C10-07C71402FFCD}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2" s="3">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBF778A-BC84-409E-B96C-156BFC05E76B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAF9DAE-C1FF-475E-AA65-DA2A164FB37F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44531A5C-67D0-468D-8D89-5AD4806882B1}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00873127-FD87-4995-841B-61152081CC1D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C17DCA-85B2-46F5-9795-1359A35BC42A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1187,18 +1599,96 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25171661-A672-4EA1-88BC-96E054E49839}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BADE4B6-7CB0-4A1A-ADF8-F242D6976257}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1335,7 +1825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1394,7 +1884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1482,7 +1972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1617,7 +2107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1676,12 +2166,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1765,7 +2253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
created commmon method to use filter; and added test filter in each module
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,41 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20348"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\eclipse-workspace\SLIIT_Automation\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF4DB0B-4A42-494A-97AF-3F8912FAD5EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="15" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
-    <sheet name="add_institute_details" sheetId="8" r:id="rId2"/>
-    <sheet name="add_new_centers" sheetId="7" r:id="rId3"/>
-    <sheet name="view_centers" sheetId="10" r:id="rId4"/>
-    <sheet name="edit_centers" sheetId="11" r:id="rId5"/>
-    <sheet name="add_new_departments" sheetId="12" r:id="rId6"/>
-    <sheet name="view_departments" sheetId="13" r:id="rId7"/>
-    <sheet name="edit_departments" sheetId="14" r:id="rId8"/>
-    <sheet name="add_new_faculty" sheetId="15" r:id="rId9"/>
-    <sheet name="add_new_awarding_institute" sheetId="16" r:id="rId10"/>
-    <sheet name="view_awarding_institutes" sheetId="17" r:id="rId11"/>
-    <sheet name="search_awarding_institute" sheetId="19" r:id="rId12"/>
-    <sheet name="edit_awarding_institute" sheetId="20" r:id="rId13"/>
-    <sheet name="add_new_classrooms" sheetId="21" r:id="rId14"/>
-    <sheet name="search_classrooms" sheetId="22" r:id="rId15"/>
-    <sheet name="view_classrooms" sheetId="28" r:id="rId16"/>
-    <sheet name="edit_classrooms" sheetId="29" r:id="rId17"/>
-    <sheet name="add_new_document_type" sheetId="23" r:id="rId18"/>
-    <sheet name="view_document_type" sheetId="25" r:id="rId19"/>
-    <sheet name="search_document_type" sheetId="24" r:id="rId20"/>
-    <sheet name="edit_document_type" sheetId="27" r:id="rId21"/>
+    <sheet name="filter_locations" sheetId="20" r:id="rId2"/>
+    <sheet name="add_institute_details" sheetId="8" r:id="rId3"/>
+    <sheet name="add_new_centers" sheetId="7" r:id="rId4"/>
+    <sheet name="filter_centers" sheetId="23" r:id="rId5"/>
+    <sheet name="view_centers" sheetId="10" r:id="rId6"/>
+    <sheet name="edit_centers" sheetId="11" r:id="rId7"/>
+    <sheet name="add_new_departments" sheetId="12" r:id="rId8"/>
+    <sheet name="filter_departments" sheetId="22" r:id="rId9"/>
+    <sheet name="view_departments" sheetId="13" r:id="rId10"/>
+    <sheet name="edit_departments" sheetId="14" r:id="rId11"/>
+    <sheet name="add_new_faculty" sheetId="15" r:id="rId12"/>
+    <sheet name="filter_faculty" sheetId="21" r:id="rId13"/>
+    <sheet name="add_new_awarding_institute" sheetId="16" r:id="rId14"/>
+    <sheet name="view_awarding_institutes" sheetId="17" r:id="rId15"/>
+    <sheet name="search_awarding_institute" sheetId="19" r:id="rId16"/>
+    <sheet name="view_classrooms" sheetId="26" r:id="rId17"/>
+    <sheet name="edit_awarding_institute" sheetId="24" r:id="rId18"/>
+    <sheet name="add_new_classrooms" sheetId="25" r:id="rId19"/>
+    <sheet name="search_classrooms" sheetId="27" r:id="rId20"/>
+    <sheet name="edit_classrooms" sheetId="28" r:id="rId21"/>
+    <sheet name="add_new_document_type" sheetId="29" r:id="rId22"/>
+    <sheet name="view_document_type" sheetId="30" r:id="rId23"/>
+    <sheet name="search_document_type" sheetId="31" r:id="rId24"/>
+    <sheet name="edit_document_type" sheetId="32" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="149">
   <si>
     <t>Y</t>
   </si>
@@ -338,24 +341,6 @@
     <t>Auto_FCT006</t>
   </si>
   <si>
-    <t>abcdefghi jklimnop 123</t>
-  </si>
-  <si>
-    <t>abcdefghi jklimnop 124</t>
-  </si>
-  <si>
-    <t>abcdefghi jklimnop 125</t>
-  </si>
-  <si>
-    <t>abcdefghi jklimnop 126</t>
-  </si>
-  <si>
-    <t>abcdefghi jklimnop 127</t>
-  </si>
-  <si>
-    <t>abcdefghi jklimnop 128</t>
-  </si>
-  <si>
     <t>Auto_AI001</t>
   </si>
   <si>
@@ -407,73 +392,115 @@
     <t>inactive</t>
   </si>
   <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Auto_FCT</t>
+  </si>
+  <si>
+    <t>Engineering_1</t>
+  </si>
+  <si>
+    <t>Engineering_2</t>
+  </si>
+  <si>
+    <t>Engineering_3</t>
+  </si>
+  <si>
+    <t>Medicine_1</t>
+  </si>
+  <si>
+    <t>Medicine_2</t>
+  </si>
+  <si>
+    <t>Medicine_3</t>
+  </si>
+  <si>
+    <t>Engine</t>
+  </si>
+  <si>
+    <t>dept</t>
+  </si>
+  <si>
+    <t>exam</t>
+  </si>
+  <si>
+    <t>CENT</t>
+  </si>
+  <si>
     <t>Auto_AI_upd_0100</t>
   </si>
   <si>
+    <t>Auto_AI_name_99</t>
+  </si>
+  <si>
     <t>Auto_AI_upd_0101</t>
   </si>
   <si>
+    <t>Auto_AI_name_100</t>
+  </si>
+  <si>
     <t>Auto_AI_upd_0102</t>
   </si>
   <si>
+    <t>Auto_AI_name_101</t>
+  </si>
+  <si>
     <t>Auto_AI_upd_0103</t>
   </si>
   <si>
-    <t>Auto_AI_name_99</t>
-  </si>
-  <si>
-    <t>Auto_AI_name_100</t>
-  </si>
-  <si>
-    <t>Auto_AI_name_101</t>
-  </si>
-  <si>
     <t>Auto_AI_name_102</t>
   </si>
   <si>
     <t>D-Block 301</t>
   </si>
   <si>
+    <t>Auto_CR_R-001</t>
+  </si>
+  <si>
+    <t>exam capacity</t>
+  </si>
+  <si>
     <t>study capacity</t>
   </si>
   <si>
-    <t>exam capacity</t>
-  </si>
-  <si>
-    <t>Auto_CR_R-001</t>
-  </si>
-  <si>
     <t>Block</t>
   </si>
   <si>
+    <t>Auto_CR_upd_0100</t>
+  </si>
+  <si>
+    <t>Auto_CR_name_99</t>
+  </si>
+  <si>
+    <t>Auto_DT_001</t>
+  </si>
+  <si>
     <t>Birth Certificate</t>
   </si>
   <si>
-    <t>Auto_DT_001</t>
-  </si>
-  <si>
     <t>Birth</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Auto_DT_upd_0100</t>
   </si>
   <si>
     <t>Auto_DT_name_99</t>
   </si>
-  <si>
-    <t>Auto_CR_upd_0100</t>
-  </si>
-  <si>
-    <t>Auto_CR_name_99</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -512,11 +539,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -797,11 +823,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +857,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -845,7 +871,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -859,7 +885,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -920,20 +946,350 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="sliit@sltnet.lk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" display="nibm@gmail.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" display="idm@idm.net" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId1" display="sliit@sltnet.lk"/>
+    <hyperlink ref="C3" r:id="rId2" display="nibm@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="idm@idm.net"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,10 +1313,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -971,10 +1327,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -985,10 +1341,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -999,10 +1355,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -1013,10 +1369,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -1030,12 +1386,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,19 +1445,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1109,34 +1465,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1144,189 +1500,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44361976-27BE-4654-ADCA-E167640F93C3}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66064CB0-35F9-4B0A-8C10-07C71402FFCD}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2">
-        <v>60</v>
-      </c>
-      <c r="D2" s="3">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBF778A-BC84-409E-B96C-156BFC05E76B}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAF9DAE-C1FF-475E-AA65-DA2A164FB37F}">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1339,15 +1514,15 @@
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1356,8 +1531,251 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44531A5C-67D0-468D-8D89-5AD4806882B1}">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1381,21 +1799,21 @@
       <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>139</v>
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1404,12 +1822,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00873127-FD87-4995-841B-61152081CC1D}">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,25 +1837,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -1451,12 +1869,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C17DCA-85B2-46F5-9795-1359A35BC42A}">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,15 +1883,15 @@
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1482,8 +1900,86 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1531,7 +2027,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1551,7 +2047,7 @@
         <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -1571,7 +2067,7 @@
         <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -1591,7 +2087,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -1599,100 +2095,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25171661-A672-4EA1-88BC-96E054E49839}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BADE4B6-7CB0-4A1A-ADF8-F242D6976257}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,8 +2242,81 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1883,8 +2374,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1971,12 +2462,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,12 +2597,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B5"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,251 +2610,69 @@
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
       <c r="B6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C6" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified test data; modified filter method to cater for skipping tests
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -428,9 +428,6 @@
     <t>Engine</t>
   </si>
   <si>
-    <t>dept</t>
-  </si>
-  <si>
     <t>exam</t>
   </si>
   <si>
@@ -495,6 +492,9 @@
   </si>
   <si>
     <t>Auto_DT_name_99</t>
+  </si>
+  <si>
+    <t>DEPT</t>
   </si>
 </sst>
 </file>
@@ -1563,10 +1563,10 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1577,10 +1577,10 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1591,10 +1591,10 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1605,10 +1605,10 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1623,7 +1623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -1643,10 +1643,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -1657,10 +1657,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2">
         <v>60</v>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
@@ -1808,10 +1808,10 @@
         <v>117</v>
       </c>
       <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1852,10 +1852,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
         <v>144</v>
-      </c>
-      <c r="B2" t="s">
-        <v>145</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
@@ -1964,10 +1964,10 @@
         <v>117</v>
       </c>
       <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2271,7 +2271,7 @@
         <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2282,7 +2282,7 @@
         <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2601,8 +2601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2626,7 +2626,7 @@
         <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
added run mode for filter test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="12" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -30,13 +30,14 @@
     <sheet name="search_awarding_institute" sheetId="19" r:id="rId16"/>
     <sheet name="view_classrooms" sheetId="26" r:id="rId17"/>
     <sheet name="edit_awarding_institute" sheetId="24" r:id="rId18"/>
-    <sheet name="add_new_classrooms" sheetId="25" r:id="rId19"/>
-    <sheet name="search_classrooms" sheetId="27" r:id="rId20"/>
-    <sheet name="edit_classrooms" sheetId="28" r:id="rId21"/>
-    <sheet name="add_new_document_type" sheetId="29" r:id="rId22"/>
-    <sheet name="view_document_type" sheetId="30" r:id="rId23"/>
-    <sheet name="search_document_type" sheetId="31" r:id="rId24"/>
-    <sheet name="edit_document_type" sheetId="32" r:id="rId25"/>
+    <sheet name="filter_awarding_institute" sheetId="33" r:id="rId19"/>
+    <sheet name="add_new_classrooms" sheetId="25" r:id="rId20"/>
+    <sheet name="search_classrooms" sheetId="27" r:id="rId21"/>
+    <sheet name="edit_classrooms" sheetId="28" r:id="rId22"/>
+    <sheet name="add_new_document_type" sheetId="29" r:id="rId23"/>
+    <sheet name="view_document_type" sheetId="30" r:id="rId24"/>
+    <sheet name="search_document_type" sheetId="31" r:id="rId25"/>
+    <sheet name="edit_document_type" sheetId="32" r:id="rId26"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="150">
   <si>
     <t>Y</t>
   </si>
@@ -495,6 +496,9 @@
   </si>
   <si>
     <t>DEPT</t>
+  </si>
+  <si>
+    <t>Auto_AI</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1293,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,6 +1624,132 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1680,70 +1810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1774,7 +1841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1822,7 +1889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1869,7 +1936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1900,7 +1967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1931,7 +1998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2601,7 +2668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified getColumnValues method to traverse the pages; debugged verifySearchResults method
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="19" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="21" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="153">
   <si>
     <t>Y</t>
   </si>
@@ -505,29 +505,20 @@
     <t>Auto_AI</t>
   </si>
   <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
     <t>z</t>
   </si>
   <si>
     <t>Computing</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>zzz</t>
+    <t>cent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +533,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF565656"/>
+      <name val="Metropolis"/>
     </font>
   </fonts>
   <fills count="2">
@@ -565,10 +561,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -857,9 +854,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -873,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -887,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -901,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -915,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -929,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -943,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -957,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -990,12 +987,12 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1003,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -1011,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -1019,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -1027,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1050,13 +1047,13 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1070,7 +1067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -1084,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -1098,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -1112,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1140,13 +1137,13 @@
       <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -1177,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -1191,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1205,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1219,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1233,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1261,12 +1258,12 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -1277,7 +1274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -1288,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>115</v>
       </c>
@@ -1299,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -1324,12 +1321,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1343,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1357,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -1371,7 +1368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -1385,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -1399,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -1427,12 +1424,12 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1440,7 +1437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -1448,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -1456,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -1464,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1487,9 +1484,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -1497,7 +1494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -1505,7 +1502,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -1513,7 +1510,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -1521,7 +1518,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -1543,9 +1540,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1553,7 +1550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -1575,12 +1572,12 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1594,7 +1591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -1608,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -1622,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -1636,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1664,12 +1661,12 @@
       <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -1680,7 +1677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -1691,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>115</v>
       </c>
@@ -1702,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -1728,12 +1725,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -1744,7 +1741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>115</v>
       </c>
@@ -1755,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>117</v>
       </c>
@@ -1766,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -1792,7 +1789,7 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -1800,7 +1797,7 @@
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1820,7 +1817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -1854,9 +1851,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -1864,7 +1861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -1886,14 +1883,14 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1907,7 +1904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -1935,13 +1932,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1955,7 +1952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -1983,9 +1980,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1993,7 +1990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -2015,9 +2012,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -2025,7 +2022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>145</v>
       </c>
@@ -2047,13 +2044,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -2067,7 +2064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -2091,13 +2088,13 @@
   <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -2105,28 +2102,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2140,12 +2137,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -2153,28 +2150,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2188,15 +2185,15 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -2204,12 +2201,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2226,14 +2223,14 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2253,7 +2250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2273,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2293,7 +2290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2313,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2350,13 +2347,13 @@
   <sheetPr codeName="Sheet30"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -2364,40 +2361,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>154</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>155</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2410,12 +2408,12 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2432,7 +2430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -2449,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2466,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -2483,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -2500,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -2517,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -2548,12 +2546,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -2564,7 +2562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -2575,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>115</v>
       </c>
@@ -2586,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -2597,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -2622,12 +2620,12 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -2635,7 +2633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -2643,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -2651,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -2659,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -2682,12 +2680,12 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -2701,7 +2699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -2715,7 +2713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -2729,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -2743,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -2771,9 +2769,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2793,7 +2791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -2813,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -2833,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -2853,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -2873,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -2907,12 +2905,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -2923,7 +2921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -2934,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>115</v>
       </c>
@@ -2945,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -2956,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -2967,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
added filter test for documenttypes; modified db clear script
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="21" activeTab="29"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="20" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -38,10 +38,11 @@
     <sheet name="view_document_type" sheetId="30" r:id="rId24"/>
     <sheet name="search_document_type" sheetId="31" r:id="rId25"/>
     <sheet name="edit_document_type" sheetId="32" r:id="rId26"/>
-    <sheet name="search_departments" sheetId="34" r:id="rId27"/>
-    <sheet name="search_centers" sheetId="35" r:id="rId28"/>
-    <sheet name="search_faculty" sheetId="36" r:id="rId29"/>
-    <sheet name="search_locations" sheetId="37" r:id="rId30"/>
+    <sheet name="filter_document_type" sheetId="38" r:id="rId27"/>
+    <sheet name="search_departments" sheetId="34" r:id="rId28"/>
+    <sheet name="search_centers" sheetId="35" r:id="rId29"/>
+    <sheet name="search_faculty" sheetId="36" r:id="rId30"/>
+    <sheet name="search_locations" sheetId="37" r:id="rId31"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="159">
   <si>
     <t>Y</t>
   </si>
@@ -484,9 +485,6 @@
     <t>Auto_CR_name_99</t>
   </si>
   <si>
-    <t>Auto_DT_001</t>
-  </si>
-  <si>
     <t>Birth Certificate</t>
   </si>
   <si>
@@ -512,6 +510,27 @@
   </si>
   <si>
     <t>cent</t>
+  </si>
+  <si>
+    <t>Auto_DT_</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>Auto_DT_004</t>
+  </si>
+  <si>
+    <t>Advanced level certiciate</t>
+  </si>
+  <si>
+    <t>Diploma certiciate</t>
+  </si>
+  <si>
+    <t>Auto_DT_005</t>
+  </si>
+  <si>
+    <t>Auto_DT_006</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1677,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1682,7 +1701,7 @@
         <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1926,10 +1945,10 @@
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1954,15 +1973,43 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
         <v>143</v>
-      </c>
-      <c r="B2" t="s">
-        <v>144</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2024,7 +2071,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
@@ -2040,7 +2087,7 @@
   <sheetPr codeName="Sheet26"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2069,10 +2116,10 @@
         <v>117</v>
       </c>
       <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2084,6 +2131,69 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:B4"/>
@@ -2131,7 +2241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet28"/>
   <dimension ref="A1:B4"/>
@@ -2160,7 +2270,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2168,44 +2278,9 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet29"/>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2344,10 +2419,45 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet29"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet30"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
@@ -2926,7 +3036,7 @@
         <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
updated classroom test cases, xpaths and test data
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\eclipse-workspace\SLIIT_Automation\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73D4261-2EBF-45D8-896A-897BCEF05266}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="20" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="17" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -19,32 +20,33 @@
     <sheet name="filter_centers" sheetId="23" r:id="rId5"/>
     <sheet name="view_centers" sheetId="10" r:id="rId6"/>
     <sheet name="edit_centers" sheetId="11" r:id="rId7"/>
-    <sheet name="add_new_departments" sheetId="12" r:id="rId8"/>
-    <sheet name="filter_departments" sheetId="22" r:id="rId9"/>
-    <sheet name="view_departments" sheetId="13" r:id="rId10"/>
-    <sheet name="edit_departments" sheetId="14" r:id="rId11"/>
-    <sheet name="add_new_faculty" sheetId="15" r:id="rId12"/>
-    <sheet name="filter_faculty" sheetId="21" r:id="rId13"/>
-    <sheet name="add_new_awarding_institute" sheetId="16" r:id="rId14"/>
-    <sheet name="view_awarding_institutes" sheetId="17" r:id="rId15"/>
-    <sheet name="search_awarding_institute" sheetId="19" r:id="rId16"/>
-    <sheet name="view_classrooms" sheetId="26" r:id="rId17"/>
-    <sheet name="edit_awarding_institute" sheetId="24" r:id="rId18"/>
-    <sheet name="filter_awarding_institute" sheetId="33" r:id="rId19"/>
-    <sheet name="add_new_classrooms" sheetId="25" r:id="rId20"/>
-    <sheet name="search_classrooms" sheetId="27" r:id="rId21"/>
-    <sheet name="edit_classrooms" sheetId="28" r:id="rId22"/>
-    <sheet name="add_new_document_type" sheetId="29" r:id="rId23"/>
-    <sheet name="view_document_type" sheetId="30" r:id="rId24"/>
-    <sheet name="search_document_type" sheetId="31" r:id="rId25"/>
-    <sheet name="edit_document_type" sheetId="32" r:id="rId26"/>
-    <sheet name="filter_document_type" sheetId="38" r:id="rId27"/>
-    <sheet name="search_departments" sheetId="34" r:id="rId28"/>
-    <sheet name="search_centers" sheetId="35" r:id="rId29"/>
-    <sheet name="search_faculty" sheetId="36" r:id="rId30"/>
-    <sheet name="search_locations" sheetId="37" r:id="rId31"/>
+    <sheet name="search_centers" sheetId="35" r:id="rId8"/>
+    <sheet name="add_new_departments" sheetId="12" r:id="rId9"/>
+    <sheet name="filter_departments" sheetId="22" r:id="rId10"/>
+    <sheet name="view_departments" sheetId="13" r:id="rId11"/>
+    <sheet name="edit_departments" sheetId="14" r:id="rId12"/>
+    <sheet name="add_new_faculty" sheetId="15" r:id="rId13"/>
+    <sheet name="filter_faculty" sheetId="21" r:id="rId14"/>
+    <sheet name="add_new_awarding_institute" sheetId="16" r:id="rId15"/>
+    <sheet name="view_awarding_institutes" sheetId="17" r:id="rId16"/>
+    <sheet name="search_awarding_institute" sheetId="19" r:id="rId17"/>
+    <sheet name="view_classrooms" sheetId="26" r:id="rId18"/>
+    <sheet name="edit_awarding_institute" sheetId="24" r:id="rId19"/>
+    <sheet name="filter_awarding_institute" sheetId="33" r:id="rId20"/>
+    <sheet name="add_new_classrooms" sheetId="25" r:id="rId21"/>
+    <sheet name="search_classrooms" sheetId="27" r:id="rId22"/>
+    <sheet name="edit_classrooms" sheetId="28" r:id="rId23"/>
+    <sheet name="filter_classrooms" sheetId="39" r:id="rId24"/>
+    <sheet name="add_new_document_type" sheetId="29" r:id="rId25"/>
+    <sheet name="view_document_type" sheetId="30" r:id="rId26"/>
+    <sheet name="search_document_type" sheetId="31" r:id="rId27"/>
+    <sheet name="edit_document_type" sheetId="32" r:id="rId28"/>
+    <sheet name="filter_document_type" sheetId="38" r:id="rId29"/>
+    <sheet name="search_departments" sheetId="34" r:id="rId30"/>
+    <sheet name="search_faculty" sheetId="36" r:id="rId31"/>
+    <sheet name="search_locations" sheetId="37" r:id="rId32"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="172">
   <si>
     <t>Y</t>
   </si>
@@ -532,11 +534,50 @@
   <si>
     <t>Auto_DT_006</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Lecture Hall</t>
+  </si>
+  <si>
+    <t>CLA</t>
+  </si>
+  <si>
+    <t>Auto_CR_R-002</t>
+  </si>
+  <si>
+    <t>D-Block 302</t>
+  </si>
+  <si>
+    <t>Computer Lab</t>
+  </si>
+  <si>
+    <t>Test center</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>new study capacity</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>new exam capacity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -580,11 +621,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -865,7 +912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -989,16 +1036,101 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="sliit@sltnet.lk"/>
-    <hyperlink ref="C3" r:id="rId2" display="nibm@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="idm@idm.net"/>
+    <hyperlink ref="C2" r:id="rId1" display="sliit@sltnet.lk" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" display="nibm@gmail.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display="idm@idm.net" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1057,8 +1189,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1147,8 +1279,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -1268,8 +1400,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1331,8 +1463,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1434,8 +1566,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1494,8 +1626,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1550,13 +1682,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1582,8 +1714,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1671,72 +1803,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet19"/>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1800,23 +1868,88 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet20"/>
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr codeName="Sheet19"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr codeName="Sheet20"/>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1824,35 +1957,82 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" t="s">
         <v>139</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>138</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>137</v>
       </c>
       <c r="B2" t="s">
         <v>136</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2">
         <v>60</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1861,8 +2041,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1893,23 +2073,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet22"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="3" max="5" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1919,11 +2099,17 @@
       <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -1933,7 +2119,13 @@
       <c r="C2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1942,8 +2134,92 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51A090-0ACB-4581-B8DF-90E1C0D51C74}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="5">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="5">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -2018,8 +2294,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2050,8 +2326,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2082,12 +2358,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr codeName="Sheet26"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2130,12 +2406,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2193,104 +2469,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet27"/>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet28"/>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -2407,10 +2587,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
@@ -2418,7 +2598,55 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <sheetPr codeName="Sheet27"/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <sheetPr codeName="Sheet29"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2452,8 +2680,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <sheetPr codeName="Sheet30"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2510,12 +2738,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2648,7 +2876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2722,7 +2950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2782,7 +3010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2871,7 +3099,55 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <sheetPr codeName="Sheet28"/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -3004,89 +3280,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added skype id in institute management and updated test data and xpaths
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73D4261-2EBF-45D8-896A-897BCEF05266}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ADA592-8C4E-4536-B7F0-DBC8998604C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="17" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="177">
   <si>
     <t>Y</t>
   </si>
@@ -572,6 +572,21 @@
   </si>
   <si>
     <t>new exam capacity</t>
+  </si>
+  <si>
+    <t>skype</t>
+  </si>
+  <si>
+    <t>sliit@skype</t>
+  </si>
+  <si>
+    <t>nibm@skype</t>
+  </si>
+  <si>
+    <t>idm@skype</t>
+  </si>
+  <si>
+    <t>acbt@skype</t>
   </si>
 </sst>
 </file>
@@ -621,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -632,6 +647,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2138,7 +2154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51A090-0ACB-4581-B8DF-90E1C0D51C74}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
@@ -2472,20 +2488,20 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="25.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2501,11 +2517,14 @@
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2521,11 +2540,14 @@
       <c r="E2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2541,11 +2563,14 @@
       <c r="E3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2561,11 +2586,14 @@
       <c r="E4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2581,7 +2609,10 @@
       <c r="E5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2591,9 +2622,13 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="F2" r:id="rId5" xr:uid="{638AF354-78A6-48E2-8245-F54BA98FFE78}"/>
+    <hyperlink ref="F3" r:id="rId6" xr:uid="{1CA9AEFA-2985-4A81-93A4-5934C1CB42DB}"/>
+    <hyperlink ref="F4" r:id="rId7" xr:uid="{4BCFC6FC-1881-4498-9774-A3171891FA8E}"/>
+    <hyperlink ref="F5" r:id="rId8" xr:uid="{B2C7B416-B629-4DB5-9ED5-BB0EF9E451B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated db delete order to support dependencies
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20349"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ADA592-8C4E-4536-B7F0-DBC8998604C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57C21C8-ED1D-4E81-91A5-3C05E24BC9D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="182">
   <si>
     <t>Y</t>
   </si>
@@ -349,36 +349,18 @@
     <t>Auto_FCT006</t>
   </si>
   <si>
-    <t>Auto_AI001</t>
-  </si>
-  <si>
-    <t>Auto_AI002</t>
-  </si>
-  <si>
-    <t>Auto_AI003</t>
-  </si>
-  <si>
-    <t>Auto_AI004</t>
-  </si>
-  <si>
     <t>Auto_AI005</t>
   </si>
   <si>
     <t>Curtin</t>
   </si>
   <si>
-    <t>Sheffield</t>
-  </si>
-  <si>
     <t>Hallam</t>
   </si>
   <si>
     <t>UGC</t>
   </si>
   <si>
-    <t>EDU</t>
-  </si>
-  <si>
     <t>+94777222222</t>
   </si>
   <si>
@@ -505,9 +487,6 @@
     <t>Auto_AI</t>
   </si>
   <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>Computing</t>
   </si>
   <si>
@@ -587,6 +566,42 @@
   </si>
   <si>
     <t>acbt@skype</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Sheffield Hallam</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Bedfordshire</t>
+  </si>
+  <si>
+    <t>LJMU</t>
+  </si>
+  <si>
+    <t>Auto_AI00811</t>
+  </si>
+  <si>
+    <t>Auto_AI00812</t>
+  </si>
+  <si>
+    <t>Auto_AI00813</t>
+  </si>
+  <si>
+    <t>Auto_AI00814</t>
+  </si>
+  <si>
+    <t>Auto_AI00815</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1091,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1087,10 +1102,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1098,7 +1113,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -1332,7 +1347,7 @@
         <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -1346,7 +1361,7 @@
         <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -1360,7 +1375,7 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -1374,7 +1389,7 @@
         <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -1388,7 +1403,7 @@
         <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
@@ -1402,7 +1417,7 @@
         <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -1432,10 +1447,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1443,10 +1458,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1454,10 +1469,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1482,18 +1497,20 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1501,84 +1518,103 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1655,7 +1691,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1663,34 +1699,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1719,7 +1755,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1763,10 +1799,10 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1777,10 +1813,10 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1791,10 +1827,10 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1805,10 +1841,10 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1835,10 +1871,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1846,7 +1882,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -1857,10 +1893,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1899,10 +1935,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1910,10 +1946,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1921,10 +1957,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1973,13 +2009,13 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F1" t="s">
         <v>90</v>
@@ -1996,13 +2032,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -2014,7 +2050,7 @@
         <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H2" t="s">
         <v>20</v>
@@ -2025,13 +2061,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -2040,10 +2076,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
@@ -2070,7 +2106,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2078,10 +2114,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2116,10 +2152,10 @@
         <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -2127,19 +2163,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -2165,10 +2201,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2176,10 +2212,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2190,7 +2226,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2265,10 +2301,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -2279,10 +2315,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -2293,10 +2329,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -2331,7 +2367,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2355,7 +2391,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2363,10 +2399,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2405,13 +2441,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2437,10 +2473,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2448,10 +2484,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2459,10 +2495,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2518,7 +2554,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -2538,10 +2574,10 @@
         <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -2561,10 +2597,10 @@
         <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
@@ -2584,10 +2620,10 @@
         <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -2607,10 +2643,10 @@
         <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
@@ -2645,7 +2681,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2669,7 +2705,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -2696,7 +2732,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2704,7 +2740,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2728,7 +2764,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2736,7 +2772,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2784,6 +2820,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2926,10 +2963,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2937,10 +2974,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2948,10 +2985,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -3136,7 +3173,7 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <sheetPr codeName="Sheet28"/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -3146,7 +3183,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3162,18 +3199,10 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3187,10 +3216,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
modified filter classroom data
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20349"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\SLIIT\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57C21C8-ED1D-4E81-91A5-3C05E24BC9D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E36BDB0-74A4-4DA3-BC53-CF59C50FB805}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5748" tabRatio="911" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="186">
   <si>
     <t>Y</t>
   </si>
@@ -602,6 +602,18 @@
   </si>
   <si>
     <t>Auto_AI00815</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -659,10 +671,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -951,7 +963,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1084,9 +1096,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1169,9 +1181,9 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1229,10 +1241,10 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1319,10 +1331,10 @@
       <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1440,9 +1452,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1503,11 +1515,11 @@
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1627,9 +1639,9 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1687,7 +1699,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1743,7 +1755,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -1775,9 +1787,9 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1864,9 +1876,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1928,9 +1940,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1992,13 +2004,13 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="5" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2102,7 +2114,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2134,11 +2146,11 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="5" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="5" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2190,20 +2202,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51A090-0ACB-4581-B8DF-90E1C0D51C74}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C1" t="s">
@@ -2214,7 +2227,7 @@
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C2" t="s">
@@ -2222,10 +2235,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C3" t="s">
@@ -2233,32 +2246,32 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="5">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5">
-        <v>60</v>
+      <c r="A4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="5">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5">
-        <v>40</v>
+      <c r="A5" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>183</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="5">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
@@ -2267,6 +2280,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2279,10 +2293,10 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2355,7 +2369,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2387,7 +2401,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2419,10 +2433,10 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2466,9 +2480,9 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2526,15 +2540,15 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="6" width="25.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.88671875" customWidth="1"/>
+    <col min="5" max="6" width="25.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2576,7 +2590,7 @@
       <c r="E2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>166</v>
       </c>
       <c r="G2" t="s">
@@ -2599,7 +2613,7 @@
       <c r="E3" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>167</v>
       </c>
       <c r="G3" t="s">
@@ -2622,7 +2636,7 @@
       <c r="E4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>168</v>
       </c>
       <c r="G4" t="s">
@@ -2645,7 +2659,7 @@
       <c r="E5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>169</v>
       </c>
       <c r="G5" t="s">
@@ -2677,7 +2691,7 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2725,7 +2739,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
@@ -2760,7 +2774,7 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2817,10 +2831,10 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2956,9 +2970,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3030,9 +3044,9 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3090,9 +3104,9 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3179,7 +3193,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3219,9 +3233,9 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
skipped data which causes indexoutofbound
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\SLIIT\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E36BDB0-74A4-4DA3-BC53-CF59C50FB805}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0297F07-854E-4B42-B557-A035A35DA582}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5748" tabRatio="911" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5748" tabRatio="911" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1223,7 +1223,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1237,8 +1237,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1314,7 +1314,7 @@
         <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2202,7 +2202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51A090-0ACB-4581-B8DF-90E1C0D51C74}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified data to fix index out of bound
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\SLIIT\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0297F07-854E-4B42-B557-A035A35DA582}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2523C9-B31C-400D-A0D0-85A788B32C1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5748" tabRatio="911" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5748" tabRatio="911" firstSheet="16" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="185">
   <si>
     <t>Y</t>
   </si>
@@ -523,9 +523,6 @@
     <t>Lecture Hall</t>
   </si>
   <si>
-    <t>CLA</t>
-  </si>
-  <si>
     <t>Auto_CR_R-002</t>
   </si>
   <si>
@@ -613,7 +610,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>8</t>
+    <t>R-005</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1234,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1530,7 +1527,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1541,13 +1538,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
         <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -1558,13 +1555,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" t="s">
         <v>172</v>
-      </c>
-      <c r="C3" t="s">
-        <v>173</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -1575,13 +1572,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -1592,13 +1589,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -1609,13 +1606,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
@@ -1636,7 +1633,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1681,7 +1678,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1784,7 +1781,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1859,7 +1856,7 @@
         <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2073,13 +2070,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" t="s">
         <v>156</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>157</v>
-      </c>
-      <c r="C3" t="s">
-        <v>158</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -2088,10 +2085,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
@@ -2164,10 +2161,10 @@
         <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -2184,10 +2181,10 @@
         <v>136</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -2202,8 +2199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51A090-0ACB-4581-B8DF-90E1C0D51C74}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2228,7 +2225,7 @@
         <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2247,10 +2244,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2258,10 +2255,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
-        <v>184</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -2269,7 +2266,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>24</v>
@@ -2568,7 +2565,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -2591,7 +2588,7 @@
         <v>101</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -2614,7 +2611,7 @@
         <v>102</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
@@ -2637,7 +2634,7 @@
         <v>103</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -2660,7 +2657,7 @@
         <v>104</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
test data for academic year
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20349"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\SLIIT\SLIIT\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CAA139-4A8A-4764-99EA-D7B3A891C1B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780C12D5-9857-4641-9301-23EA8B288CC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5748" tabRatio="911" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="26" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -45,6 +45,8 @@
     <sheet name="search_departments" sheetId="34" r:id="rId30"/>
     <sheet name="search_faculty" sheetId="36" r:id="rId31"/>
     <sheet name="search_locations" sheetId="37" r:id="rId32"/>
+    <sheet name="add_new_academic_year" sheetId="40" r:id="rId33"/>
+    <sheet name="search_academic_years" sheetId="41" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="195">
   <si>
     <t>Y</t>
   </si>
@@ -611,6 +613,36 @@
   </si>
   <si>
     <t>R-005</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>awarding institute</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>Faculty of Engineering</t>
+  </si>
+  <si>
+    <t>2023-2024</t>
+  </si>
+  <si>
+    <t>Auto_AY_2023-2024 academic year for Engineering fac</t>
+  </si>
+  <si>
+    <t>Auto_AY_2022-2023 academic year for Engineering fac</t>
+  </si>
+  <si>
+    <t>2022-</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
   </si>
 </sst>
 </file>
@@ -660,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -671,6 +703,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -960,7 +995,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1093,9 +1128,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1178,9 +1213,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1238,10 +1273,10 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1328,10 +1363,10 @@
       <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1449,9 +1484,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1512,11 +1547,11 @@
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1632,13 +1667,13 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1696,7 +1731,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1752,7 +1787,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -1784,9 +1819,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1873,9 +1908,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1937,9 +1972,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2001,13 +2036,13 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="7" width="13.88671875" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2111,7 +2146,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2143,11 +2178,11 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="5" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="5" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2203,10 +2238,10 @@
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2287,13 +2322,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2366,7 +2401,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2398,7 +2433,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2430,10 +2465,10 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2477,9 +2512,9 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2541,11 +2576,11 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="45.88671875" customWidth="1"/>
-    <col min="5" max="6" width="25.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="6" width="25.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2685,10 +2720,10 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2736,7 +2771,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
@@ -2771,7 +2806,7 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2816,6 +2851,141 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715FC5D-711D-45AE-936E-840A2F2438E3}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="7" customFormat="1" ht="30">
+      <c r="A2" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="7" customFormat="1" ht="30">
+      <c r="A3" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F61D29-2E90-40EC-B5CF-57C9936653DE}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2828,10 +2998,10 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2967,9 +3137,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3041,9 +3211,9 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3101,9 +3271,9 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3190,7 +3360,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3230,9 +3400,9 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Program types - test cases, testing.xml, testdata and or.properties
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20349"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20350"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE88C7A-2734-4020-A432-A3E1E09C04D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAB022E-5E94-4D51-8AD5-6352D7829DFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="30" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="34" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -50,6 +50,11 @@
     <sheet name="view_academic_years" sheetId="42" r:id="rId35"/>
     <sheet name="edit_academic_years" sheetId="43" r:id="rId36"/>
     <sheet name="filter_academic_years" sheetId="44" r:id="rId37"/>
+    <sheet name="add_new_program_types" sheetId="45" r:id="rId38"/>
+    <sheet name="edit_program_types" sheetId="46" r:id="rId39"/>
+    <sheet name="view_program_types" sheetId="47" r:id="rId40"/>
+    <sheet name="filter_program_types" sheetId="49" r:id="rId41"/>
+    <sheet name="search_program_types" sheetId="48" r:id="rId42"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="220">
   <si>
     <t>Y</t>
   </si>
@@ -673,6 +678,54 @@
   </si>
   <si>
     <t>2019-2021</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Bachelors degree</t>
+  </si>
+  <si>
+    <t>Auto_PT_001</t>
+  </si>
+  <si>
+    <t>Auto_PT_002</t>
+  </si>
+  <si>
+    <t>Short courses</t>
+  </si>
+  <si>
+    <t>aptitude</t>
+  </si>
+  <si>
+    <t>research proposal</t>
+  </si>
+  <si>
+    <t>interview</t>
+  </si>
+  <si>
+    <t>Auto_UPD_PT_001</t>
+  </si>
+  <si>
+    <t>Auto_UPD_PT_002</t>
+  </si>
+  <si>
+    <t>UPD_Degree</t>
+  </si>
+  <si>
+    <t>UPD_Short courses</t>
+  </si>
+  <si>
+    <t>UPD_Bachelors degree</t>
+  </si>
+  <si>
+    <t>PT_001</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Not Required</t>
   </si>
 </sst>
 </file>
@@ -2889,7 +2942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715FC5D-711D-45AE-936E-840A2F2438E3}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2976,7 +3029,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3124,7 +3177,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3173,6 +3226,202 @@
         <v>200</v>
       </c>
       <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D62FA9-201D-4EC6-B6B9-E567E0D0C68A}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A8DA1A-9954-44E9-A216-001A153ECDB1}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3320,6 +3569,179 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1639AC-EB0B-409F-A9B4-9EEA30E89A15}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FCBFFB-22A6-4482-83BD-FC8630938E34}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF7A2C6-9D8C-4CC5-AD2C-948B8E95011F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>

</xml_diff>

<commit_message>
Qualification types,testdata. testing.xml & xapths
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81106AC-04B9-47E9-9FA0-CF9493133BAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C7BAF9-512E-49B9-B730-BFF43DF3E585}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="34" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="45" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -55,6 +55,11 @@
     <sheet name="view_program_types" sheetId="47" r:id="rId40"/>
     <sheet name="filter_program_types" sheetId="49" r:id="rId41"/>
     <sheet name="search_program_types" sheetId="48" r:id="rId42"/>
+    <sheet name="add_new_qualification_types" sheetId="50" r:id="rId43"/>
+    <sheet name="search_qualification_types" sheetId="51" r:id="rId44"/>
+    <sheet name="view_qualification_types" sheetId="52" r:id="rId45"/>
+    <sheet name="filter_qualification_types" sheetId="53" r:id="rId46"/>
+    <sheet name="edit_qualification_types" sheetId="54" r:id="rId47"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="243">
   <si>
     <t>Y</t>
   </si>
@@ -125,9 +130,6 @@
     <t>Jaffna</t>
   </si>
   <si>
-    <t>Gall</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
@@ -137,9 +139,6 @@
     <t>Kandy</t>
   </si>
   <si>
-    <t>Jaela</t>
-  </si>
-  <si>
     <t>Inactive</t>
   </si>
   <si>
@@ -173,15 +172,6 @@
     <t>library</t>
   </si>
   <si>
-    <t>canteen</t>
-  </si>
-  <si>
-    <t>recreation area</t>
-  </si>
-  <si>
-    <t>wash room</t>
-  </si>
-  <si>
     <t>row</t>
   </si>
   <si>
@@ -203,9 +193,6 @@
     <t>new name</t>
   </si>
   <si>
-    <t>Kalutara2</t>
-  </si>
-  <si>
     <t>sliit@slt.net</t>
   </si>
   <si>
@@ -726,6 +713,93 @@
   </si>
   <si>
     <t>Not Required</t>
+  </si>
+  <si>
+    <t>Auto_QT_001</t>
+  </si>
+  <si>
+    <t>Auto_QT_002</t>
+  </si>
+  <si>
+    <t>QT_001</t>
+  </si>
+  <si>
+    <t>Auto_UPD_QT_001</t>
+  </si>
+  <si>
+    <t>Auto_UPD_QT_002</t>
+  </si>
+  <si>
+    <t>Sri Lankan A/L</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Sri Lankan O/L</t>
+  </si>
+  <si>
+    <t>UPD_Sri Lankan A/L</t>
+  </si>
+  <si>
+    <t>UPD_Sri Lankan O/L</t>
+  </si>
+  <si>
+    <t>UPD_Mathematics</t>
+  </si>
+  <si>
+    <t>outcome1</t>
+  </si>
+  <si>
+    <t>outcome2</t>
+  </si>
+  <si>
+    <t>Combined Maths</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>new outcome1</t>
+  </si>
+  <si>
+    <t>A/L</t>
+  </si>
+  <si>
+    <t>UPD_Physics</t>
+  </si>
+  <si>
+    <t>Kandy city campus</t>
+  </si>
+  <si>
+    <t>Matara</t>
+  </si>
+  <si>
+    <t>Matara city</t>
+  </si>
+  <si>
+    <t>Malabe campus</t>
+  </si>
+  <si>
+    <t>Metro</t>
+  </si>
+  <si>
+    <t>Kolpity</t>
+  </si>
+  <si>
+    <t>Malabe</t>
+  </si>
+  <si>
+    <t>Jaffna campus</t>
+  </si>
+  <si>
+    <t>Jaffna city</t>
+  </si>
+  <si>
+    <t>Auto_QT</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1150,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1097,13 +1171,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1111,13 +1185,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1125,13 +1199,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1139,13 +1213,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1153,13 +1227,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1167,13 +1241,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>238</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1181,13 +1255,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>239</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -1219,10 +1293,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1230,10 +1304,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1241,10 +1315,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1252,10 +1326,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -1263,10 +1337,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -1274,10 +1348,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1304,7 +1378,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1312,7 +1386,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1320,7 +1394,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1328,7 +1402,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1336,7 +1410,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1365,13 +1439,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1379,13 +1453,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1393,13 +1467,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1407,13 +1481,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1421,13 +1495,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -1461,7 +1535,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1472,13 +1546,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1486,13 +1560,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -1500,13 +1574,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -1514,13 +1588,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -1528,13 +1602,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -1542,13 +1616,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
@@ -1575,10 +1649,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1586,10 +1660,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1597,10 +1671,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1608,10 +1682,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -1646,7 +1720,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1657,16 +1731,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1674,16 +1748,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -1691,16 +1765,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -1708,16 +1782,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -1725,16 +1799,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -1762,7 +1836,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1770,7 +1844,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1778,7 +1852,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1786,7 +1860,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1794,7 +1868,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1819,7 +1893,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1827,34 +1901,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
         <v>100</v>
-      </c>
-      <c r="B4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1875,7 +1949,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1883,7 +1957,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1910,13 +1984,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1924,13 +1998,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1938,13 +2012,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1952,13 +2026,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1966,13 +2040,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -1999,10 +2073,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2010,10 +2084,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2021,10 +2095,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2032,10 +2106,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2063,10 +2137,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2074,10 +2148,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2085,10 +2159,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2096,10 +2170,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2137,19 +2211,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
         <v>16</v>
@@ -2160,13 +2234,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -2175,13 +2249,13 @@
         <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
@@ -2189,13 +2263,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -2204,13 +2278,13 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
         <v>0</v>
@@ -2234,7 +2308,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2242,10 +2316,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2271,19 +2345,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -2291,19 +2365,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -2330,10 +2404,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2341,10 +2415,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2352,10 +2426,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2363,10 +2437,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2374,10 +2448,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -2385,10 +2459,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -2431,13 +2505,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2445,13 +2519,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2459,13 +2533,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2489,7 +2563,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2497,7 +2571,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2521,7 +2595,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2529,10 +2603,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2557,13 +2631,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2571,13 +2645,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2603,10 +2677,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2614,10 +2688,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2625,10 +2699,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2636,10 +2710,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2678,13 +2752,13 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -2698,16 +2772,16 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -2724,13 +2798,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
@@ -2747,13 +2821,13 @@
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -2761,22 +2835,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
@@ -2811,7 +2885,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2819,7 +2893,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2827,7 +2901,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2835,7 +2909,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -2862,7 +2936,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2870,7 +2944,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2894,7 +2968,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2902,7 +2976,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2910,7 +2984,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2918,7 +2992,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -2926,7 +3000,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2955,22 +3029,22 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G1" t="s">
         <v>16</v>
@@ -2981,19 +3055,19 @@
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A2" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -3001,19 +3075,19 @@
     </row>
     <row r="3" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A3" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
         <v>0</v>
@@ -3036,7 +3110,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3044,7 +3118,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3052,7 +3126,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3060,7 +3134,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3068,7 +3142,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -3091,7 +3165,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3099,7 +3173,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3126,13 +3200,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3140,13 +3214,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3154,13 +3228,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3187,10 +3261,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3198,10 +3272,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -3209,10 +3283,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -3220,10 +3294,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -3239,7 +3313,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3257,19 +3331,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="G1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -3277,16 +3351,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -3303,16 +3377,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -3337,7 +3411,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3349,25 +3423,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="G1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -3375,16 +3449,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -3401,16 +3475,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -3436,12 +3510,13 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3453,7 +3528,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -3464,16 +3539,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>236</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -3481,16 +3556,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>237</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>238</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -3498,16 +3573,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -3515,16 +3590,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>235</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>234</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -3532,16 +3607,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>240</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -3549,16 +3624,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>233</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
@@ -3573,15 +3648,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1639AC-EB0B-409F-A9B4-9EEA30E89A15}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3589,7 +3664,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3597,7 +3672,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3613,7 +3688,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3623,10 +3698,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3634,10 +3709,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -3645,10 +3720,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -3656,10 +3731,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -3667,10 +3742,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -3678,10 +3753,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -3697,7 +3772,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3707,7 +3782,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3715,7 +3790,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3723,7 +3798,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3731,9 +3806,297 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DC2690-2472-400B-9B25-29E91FDA57F0}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="4" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E830D701-6D8C-4359-83F5-87DCB34EC8B9}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD734D45-0559-4EC2-8E5B-ACF2C7B6FD86}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C55E90-6AE9-483F-8DA0-C3CF954979F9}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14DE688-905A-4831-96B7-270AE5C33133}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3758,10 +4121,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3769,10 +4132,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -3780,10 +4143,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -3791,10 +4154,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -3802,10 +4165,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -3832,7 +4195,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3840,7 +4203,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3848,7 +4211,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3856,7 +4219,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3864,7 +4227,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -3887,18 +4250,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3906,13 +4270,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3920,13 +4284,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3934,13 +4298,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -3948,13 +4312,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -3978,7 +4342,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3986,7 +4350,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3994,7 +4358,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4027,10 +4391,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -4041,19 +4405,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -4061,19 +4425,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -4081,19 +4445,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -4101,19 +4465,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -4121,19 +4485,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Revert "Qualification types & DB script"
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C7BAF9-512E-49B9-B730-BFF43DF3E585}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81106AC-04B9-47E9-9FA0-CF9493133BAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="45" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="34" activeTab="39" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -55,11 +55,6 @@
     <sheet name="view_program_types" sheetId="47" r:id="rId40"/>
     <sheet name="filter_program_types" sheetId="49" r:id="rId41"/>
     <sheet name="search_program_types" sheetId="48" r:id="rId42"/>
-    <sheet name="add_new_qualification_types" sheetId="50" r:id="rId43"/>
-    <sheet name="search_qualification_types" sheetId="51" r:id="rId44"/>
-    <sheet name="view_qualification_types" sheetId="52" r:id="rId45"/>
-    <sheet name="filter_qualification_types" sheetId="53" r:id="rId46"/>
-    <sheet name="edit_qualification_types" sheetId="54" r:id="rId47"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="220">
   <si>
     <t>Y</t>
   </si>
@@ -130,6 +125,9 @@
     <t>Jaffna</t>
   </si>
   <si>
+    <t>Gall</t>
+  </si>
+  <si>
     <t>Active</t>
   </si>
   <si>
@@ -139,6 +137,9 @@
     <t>Kandy</t>
   </si>
   <si>
+    <t>Jaela</t>
+  </si>
+  <si>
     <t>Inactive</t>
   </si>
   <si>
@@ -172,6 +173,15 @@
     <t>library</t>
   </si>
   <si>
+    <t>canteen</t>
+  </si>
+  <si>
+    <t>recreation area</t>
+  </si>
+  <si>
+    <t>wash room</t>
+  </si>
+  <si>
     <t>row</t>
   </si>
   <si>
@@ -193,6 +203,9 @@
     <t>new name</t>
   </si>
   <si>
+    <t>Kalutara2</t>
+  </si>
+  <si>
     <t>sliit@slt.net</t>
   </si>
   <si>
@@ -713,93 +726,6 @@
   </si>
   <si>
     <t>Not Required</t>
-  </si>
-  <si>
-    <t>Auto_QT_001</t>
-  </si>
-  <si>
-    <t>Auto_QT_002</t>
-  </si>
-  <si>
-    <t>QT_001</t>
-  </si>
-  <si>
-    <t>Auto_UPD_QT_001</t>
-  </si>
-  <si>
-    <t>Auto_UPD_QT_002</t>
-  </si>
-  <si>
-    <t>Sri Lankan A/L</t>
-  </si>
-  <si>
-    <t>Maths</t>
-  </si>
-  <si>
-    <t>Sri Lankan O/L</t>
-  </si>
-  <si>
-    <t>UPD_Sri Lankan A/L</t>
-  </si>
-  <si>
-    <t>UPD_Sri Lankan O/L</t>
-  </si>
-  <si>
-    <t>UPD_Mathematics</t>
-  </si>
-  <si>
-    <t>outcome1</t>
-  </si>
-  <si>
-    <t>outcome2</t>
-  </si>
-  <si>
-    <t>Combined Maths</t>
-  </si>
-  <si>
-    <t>Chemistry</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>new outcome1</t>
-  </si>
-  <si>
-    <t>A/L</t>
-  </si>
-  <si>
-    <t>UPD_Physics</t>
-  </si>
-  <si>
-    <t>Kandy city campus</t>
-  </si>
-  <si>
-    <t>Matara</t>
-  </si>
-  <si>
-    <t>Matara city</t>
-  </si>
-  <si>
-    <t>Malabe campus</t>
-  </si>
-  <si>
-    <t>Metro</t>
-  </si>
-  <si>
-    <t>Kolpity</t>
-  </si>
-  <si>
-    <t>Malabe</t>
-  </si>
-  <si>
-    <t>Jaffna campus</t>
-  </si>
-  <si>
-    <t>Jaffna city</t>
-  </si>
-  <si>
-    <t>Auto_QT</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1076,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1171,13 +1097,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1185,13 +1111,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1199,13 +1125,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1213,13 +1139,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1227,13 +1153,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1241,13 +1167,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1255,13 +1181,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>239</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -1293,10 +1219,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1304,10 +1230,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1315,10 +1241,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1326,10 +1252,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -1337,10 +1263,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -1348,10 +1274,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1378,7 +1304,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1386,7 +1312,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1394,7 +1320,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1402,7 +1328,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1410,7 +1336,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1439,13 +1365,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1453,13 +1379,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1467,13 +1393,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1481,13 +1407,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1495,13 +1421,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -1535,7 +1461,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1546,13 +1472,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1560,13 +1486,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -1574,13 +1500,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -1588,13 +1514,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -1602,13 +1528,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -1616,13 +1542,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
@@ -1649,10 +1575,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1660,10 +1586,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1671,10 +1597,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1682,10 +1608,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -1720,7 +1646,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1731,16 +1657,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
         <v>170</v>
       </c>
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>164</v>
-      </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1748,16 +1674,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="s">
         <v>171</v>
       </c>
-      <c r="B3" t="s">
-        <v>165</v>
-      </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -1765,16 +1691,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -1782,16 +1708,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -1799,16 +1725,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -1836,7 +1762,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1844,7 +1770,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1852,7 +1778,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1860,7 +1786,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1868,7 +1794,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1893,7 +1819,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1901,34 +1827,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1949,7 +1875,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1957,7 +1883,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1984,13 +1910,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1998,13 +1924,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2012,13 +1938,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2026,13 +1952,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2040,13 +1966,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -2073,10 +1999,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2084,10 +2010,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2095,10 +2021,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2106,10 +2032,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2137,10 +2063,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2148,10 +2074,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2159,10 +2085,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2170,10 +2096,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2211,19 +2137,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
         <v>16</v>
@@ -2234,13 +2160,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -2249,13 +2175,13 @@
         <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
@@ -2263,13 +2189,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -2278,13 +2204,13 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
         <v>0</v>
@@ -2308,7 +2234,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2316,10 +2242,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2345,19 +2271,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -2365,19 +2291,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -2404,10 +2330,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2415,10 +2341,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2426,10 +2352,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2437,10 +2363,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2448,10 +2374,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -2459,10 +2385,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -2505,13 +2431,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2519,13 +2445,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2533,13 +2459,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2563,7 +2489,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2571,7 +2497,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2595,7 +2521,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2603,10 +2529,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2631,13 +2557,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2645,13 +2571,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2677,10 +2603,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2688,10 +2614,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2699,10 +2625,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2710,10 +2636,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2752,13 +2678,13 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -2772,16 +2698,16 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -2798,13 +2724,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
@@ -2821,13 +2747,13 @@
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -2835,22 +2761,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
@@ -2885,7 +2811,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2893,7 +2819,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2901,7 +2827,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2909,7 +2835,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -2936,7 +2862,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2944,7 +2870,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2968,7 +2894,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2976,7 +2902,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2984,7 +2910,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2992,7 +2918,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3000,7 +2926,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -3029,22 +2955,22 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="E1" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="F1" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="G1" t="s">
         <v>16</v>
@@ -3055,19 +2981,19 @@
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A2" s="7" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -3075,19 +3001,19 @@
     </row>
     <row r="3" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A3" s="7" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
         <v>0</v>
@@ -3110,7 +3036,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3118,7 +3044,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3126,7 +3052,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3134,7 +3060,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3142,7 +3068,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -3165,7 +3091,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3173,7 +3099,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3200,13 +3126,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3214,13 +3140,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3228,13 +3154,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3261,10 +3187,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3272,10 +3198,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -3283,10 +3209,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -3294,10 +3220,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -3313,7 +3239,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3331,19 +3257,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -3351,16 +3277,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -3377,16 +3303,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -3411,7 +3337,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3423,25 +3349,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -3449,16 +3375,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C2" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -3475,16 +3401,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="D3" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -3510,13 +3436,12 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3528,7 +3453,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -3539,16 +3464,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>239</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -3556,16 +3481,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -3573,16 +3498,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>241</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
@@ -3590,16 +3515,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -3607,16 +3532,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>240</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -3624,16 +3549,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
@@ -3648,15 +3573,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1639AC-EB0B-409F-A9B4-9EEA30E89A15}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3664,7 +3589,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3672,7 +3597,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3688,7 +3613,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3698,10 +3623,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3709,10 +3634,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -3720,10 +3645,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -3731,10 +3656,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -3742,10 +3667,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -3753,10 +3678,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -3772,7 +3697,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3782,7 +3707,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3790,7 +3715,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3798,7 +3723,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3806,297 +3731,9 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DC2690-2472-400B-9B25-29E91FDA57F0}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="4" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E830D701-6D8C-4359-83F5-87DCB34EC8B9}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD734D45-0559-4EC2-8E5B-ACF2C7B6FD86}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C55E90-6AE9-483F-8DA0-C3CF954979F9}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14DE688-905A-4831-96B7-270AE5C33133}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4121,10 +3758,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -4132,10 +3769,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -4143,10 +3780,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -4154,10 +3791,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -4165,10 +3802,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -4195,7 +3832,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4203,7 +3840,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4211,7 +3848,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4219,7 +3856,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -4227,7 +3864,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -4250,19 +3887,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -4270,13 +3906,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -4284,13 +3920,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -4298,13 +3934,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -4312,13 +3948,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -4342,7 +3978,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4350,7 +3986,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4358,7 +3994,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4391,10 +4027,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -4405,19 +4041,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -4425,19 +4061,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -4445,19 +4081,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
@@ -4465,19 +4101,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -4485,19 +4121,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Asessment criteria and qualification types
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C7BAF9-512E-49B9-B730-BFF43DF3E585}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738CAC31-CD11-4133-937F-1B7C7ABC92B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="45" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="45" activeTab="51" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -60,6 +60,11 @@
     <sheet name="view_qualification_types" sheetId="52" r:id="rId45"/>
     <sheet name="filter_qualification_types" sheetId="53" r:id="rId46"/>
     <sheet name="edit_qualification_types" sheetId="54" r:id="rId47"/>
+    <sheet name="add_new_assessment_criteria" sheetId="55" r:id="rId48"/>
+    <sheet name="search_assessment_criteria" sheetId="56" r:id="rId49"/>
+    <sheet name="view_assessment_criteria" sheetId="57" r:id="rId50"/>
+    <sheet name="filter_assessment_criteria" sheetId="58" r:id="rId51"/>
+    <sheet name="edit_assessment_criteria" sheetId="59" r:id="rId52"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="261">
   <si>
     <t>Y</t>
   </si>
@@ -800,6 +805,60 @@
   </si>
   <si>
     <t>Auto_QT</t>
+  </si>
+  <si>
+    <t>Auto_AC_001</t>
+  </si>
+  <si>
+    <t>Auto_AC_002</t>
+  </si>
+  <si>
+    <t>sub assessment1</t>
+  </si>
+  <si>
+    <t>sub assessment2</t>
+  </si>
+  <si>
+    <t>Final Exam</t>
+  </si>
+  <si>
+    <t>Theory</t>
+  </si>
+  <si>
+    <t>Viva</t>
+  </si>
+  <si>
+    <t>Mid Exam</t>
+  </si>
+  <si>
+    <t>Auto_UPD_AC_001</t>
+  </si>
+  <si>
+    <t>Auto_UPD_AC_002</t>
+  </si>
+  <si>
+    <t>UPD_Final Exam</t>
+  </si>
+  <si>
+    <t>UPD_Mid Exam</t>
+  </si>
+  <si>
+    <t>AC_001</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Auto_AC</t>
+  </si>
+  <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>new sub assessment</t>
+  </si>
+  <si>
+    <t>Lab</t>
   </si>
 </sst>
 </file>
@@ -3822,7 +3881,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3886,7 +3945,7 @@
         <v>229</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -3902,7 +3961,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3949,7 +4008,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3987,8 +4046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C55E90-6AE9-483F-8DA0-C3CF954979F9}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4039,7 +4098,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4105,6 +4164,126 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336AC193-3915-4484-8D65-F7E4A363C2FB}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8139E5A-5F8E-4113-B2AF-9C94BF152E85}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
@@ -4179,6 +4358,164 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8AC81F-BE3D-4D4E-B606-C922D904C76D}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E42928-E64E-4568-B02E-7237A836E7A6}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265B421F-608A-417E-BE3C-DE35E0891BE7}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>

</xml_diff>

<commit_message>
entry criteria - add
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08724EB4-0AE2-478C-B1AF-5DCED76CD976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7563F1-B870-4FE7-BF3A-456AAB9FEFD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="52" activeTab="54" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="42" activeTab="47" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -60,16 +60,17 @@
     <sheet name="view_qualification_types" sheetId="52" r:id="rId45"/>
     <sheet name="filter_qualification_types" sheetId="53" r:id="rId46"/>
     <sheet name="edit_qualification_types" sheetId="54" r:id="rId47"/>
-    <sheet name="add_new_assessment_criteria" sheetId="55" r:id="rId48"/>
-    <sheet name="search_assessment_criteria" sheetId="56" r:id="rId49"/>
-    <sheet name="view_assessment_criteria" sheetId="57" r:id="rId50"/>
-    <sheet name="filter_assessment_criteria" sheetId="58" r:id="rId51"/>
-    <sheet name="edit_assessment_criteria" sheetId="59" r:id="rId52"/>
-    <sheet name="add_new_learning_outcomes" sheetId="61" r:id="rId53"/>
-    <sheet name="search_learning_outcomes" sheetId="62" r:id="rId54"/>
-    <sheet name="view_learning_outcomes" sheetId="63" r:id="rId55"/>
-    <sheet name="filter_learning_outcomes" sheetId="64" r:id="rId56"/>
-    <sheet name="edit_learning_outcomes" sheetId="60" r:id="rId57"/>
+    <sheet name="add_new_entry_criteria" sheetId="65" r:id="rId48"/>
+    <sheet name="add_new_assessment_criteria" sheetId="55" r:id="rId49"/>
+    <sheet name="search_assessment_criteria" sheetId="56" r:id="rId50"/>
+    <sheet name="view_assessment_criteria" sheetId="57" r:id="rId51"/>
+    <sheet name="filter_assessment_criteria" sheetId="58" r:id="rId52"/>
+    <sheet name="edit_assessment_criteria" sheetId="59" r:id="rId53"/>
+    <sheet name="add_new_learning_outcomes" sheetId="61" r:id="rId54"/>
+    <sheet name="search_learning_outcomes" sheetId="62" r:id="rId55"/>
+    <sheet name="view_learning_outcomes" sheetId="63" r:id="rId56"/>
+    <sheet name="filter_learning_outcomes" sheetId="64" r:id="rId57"/>
+    <sheet name="edit_learning_outcomes" sheetId="60" r:id="rId58"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="279">
   <si>
     <t>Y</t>
   </si>
@@ -894,6 +895,30 @@
   </si>
   <si>
     <t>_LCO_00</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>subject1</t>
+  </si>
+  <si>
+    <t>subject2</t>
+  </si>
+  <si>
+    <t>result1</t>
+  </si>
+  <si>
+    <t>Combined maths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A </t>
+  </si>
+  <si>
+    <t>Auto_Sri Lankan A/L</t>
+  </si>
+  <si>
+    <t>Auto_EC_001</t>
   </si>
 </sst>
 </file>
@@ -943,7 +968,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -959,6 +984,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3415,7 +3443,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3513,7 +3541,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3924,14 +3952,15 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="4" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4208,6 +4237,78 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E778355F-ADB3-4B6B-9F8B-BC08BD69B35F}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="26.25" customHeight="1"/>
+    <row r="9" spans="1:8" ht="26.25" customHeight="1"/>
+    <row r="10" spans="1:8" ht="26.25" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336AC193-3915-4484-8D65-F7E4A363C2FB}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -4288,45 +4389,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8139E5A-5F8E-4113-B2AF-9C94BF152E85}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
@@ -4402,6 +4464,45 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8139E5A-5F8E-4113-B2AF-9C94BF152E85}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8AC81F-BE3D-4D4E-B606-C922D904C76D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4440,7 +4541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E42928-E64E-4568-B02E-7237A836E7A6}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -4488,7 +4589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265B421F-608A-417E-BE3C-DE35E0891BE7}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -4559,7 +4660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309BBC27-0FD6-4321-B6C5-A8F361F2CAF6}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -4631,7 +4732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF6E375-E7B8-4284-B72D-D9C5E9349A84}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4673,11 +4774,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6844A23B-4865-4BC7-8285-CA3C17CB7B4E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -4712,7 +4813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A48781E-2C8F-4AF6-A17E-4002F5DCF3F3}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -4763,7 +4864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6832BC4F-C2E1-46D9-80A8-A3A62DC2CD40}">
   <dimension ref="A1:D3"/>
   <sheetViews>

</xml_diff>

<commit_message>
entry criteria add and edit
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BE757A-51A2-4E17-85D4-058E1079E1FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3724A03F-4350-4E9F-B063-7D9D556904CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="59" activeTab="65" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="44" activeTab="51" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="320">
   <si>
     <t>Y</t>
   </si>
@@ -1033,6 +1033,24 @@
   </si>
   <si>
     <t>BSc</t>
+  </si>
+  <si>
+    <t>new type</t>
+  </si>
+  <si>
+    <t>new outcome</t>
+  </si>
+  <si>
+    <t>London A/L</t>
+  </si>
+  <si>
+    <t>new grade</t>
+  </si>
+  <si>
+    <t>new value</t>
+  </si>
+  <si>
+    <t>bio</t>
   </si>
 </sst>
 </file>
@@ -4066,7 +4084,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4284,7 +4302,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4352,10 +4370,10 @@
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E778355F-ADB3-4B6B-9F8B-BC08BD69B35F}">
-  <dimension ref="A1:N10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4366,8 +4384,8 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="9" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="9" customWidth="1"/>
+    <col min="12" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4466,9 +4484,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="26.25" customHeight="1"/>
-    <row r="9" spans="1:10" ht="26.25" customHeight="1"/>
-    <row r="10" spans="1:10" ht="26.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4479,7 +4494,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4676,19 +4691,22 @@
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923C27E3-C15F-465A-8C31-E4DAE8B30273}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -4699,61 +4717,79 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" t="s">
         <v>289</v>
       </c>
-      <c r="E1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F1" t="s">
-        <v>281</v>
-      </c>
       <c r="G1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>317</v>
+      </c>
+      <c r="H1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="D2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" t="s">
         <v>224</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>288</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C3" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="D3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F3" t="s">
         <v>224</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>288</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5558,7 +5594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9F3390-C4DC-438C-93B1-4FBC35E51A49}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add more tests for subject
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\SLIIT\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08724EB4-0AE2-478C-B1AF-5DCED76CD976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0395DC7D-292E-456C-A270-483C1160F48F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="52" activeTab="54" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9242" windowHeight="5747" tabRatio="911" firstSheet="53" activeTab="58" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -70,6 +70,8 @@
     <sheet name="view_learning_outcomes" sheetId="63" r:id="rId55"/>
     <sheet name="filter_learning_outcomes" sheetId="64" r:id="rId56"/>
     <sheet name="edit_learning_outcomes" sheetId="60" r:id="rId57"/>
+    <sheet name="add_subjects" sheetId="65" r:id="rId58"/>
+    <sheet name="filterSubjects" sheetId="66" r:id="rId59"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="289">
   <si>
     <t>Y</t>
   </si>
@@ -894,6 +896,60 @@
   </si>
   <si>
     <t>_LCO_00</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>dept</t>
+  </si>
+  <si>
+    <t>Auto_SBJ_001</t>
+  </si>
+  <si>
+    <t>Auto_SBJ_002</t>
+  </si>
+  <si>
+    <t>Auto_SBJ_003</t>
+  </si>
+  <si>
+    <t>sessioncode</t>
+  </si>
+  <si>
+    <t>sessionname</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>sub001</t>
+  </si>
+  <si>
+    <t>sub002</t>
+  </si>
+  <si>
+    <t>sub003</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>thrid</t>
+  </si>
+  <si>
+    <t>SUN03</t>
+  </si>
+  <si>
+    <t>Computer</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1303,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1380,9 +1436,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1465,9 +1521,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1525,10 +1581,10 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1615,10 +1671,10 @@
       <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1736,9 +1792,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1799,11 +1855,11 @@
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1923,9 +1979,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1983,7 +2039,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2039,7 +2095,7 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2079,9 +2135,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2168,9 +2224,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2232,9 +2288,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2296,13 +2352,13 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="5" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2406,7 +2462,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2438,11 +2494,11 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="5" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="5" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2498,10 +2554,10 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2585,10 +2641,10 @@
       <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2661,7 +2717,7 @@
       <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2693,7 +2749,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2725,10 +2781,10 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2772,9 +2828,9 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2836,11 +2892,11 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="6" width="25.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.88671875" customWidth="1"/>
+    <col min="5" max="6" width="25.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2983,7 +3039,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3031,7 +3087,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
@@ -3066,7 +3122,7 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3122,10 +3178,10 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
     <col min="4" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3155,7 +3211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="30">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="30.15">
       <c r="A2" s="7" t="s">
         <v>182</v>
       </c>
@@ -3175,7 +3231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="30">
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="30.15">
       <c r="A3" s="7" t="s">
         <v>184</v>
       </c>
@@ -3208,7 +3264,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3263,7 +3319,7 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -3294,10 +3350,10 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3356,9 +3412,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3418,10 +3474,10 @@
       <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3516,11 +3572,11 @@
       <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3615,11 +3671,11 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3754,7 +3810,7 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3793,9 +3849,9 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3877,7 +3933,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
@@ -3927,11 +3983,11 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="4" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="4" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4007,7 +4063,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4054,7 +4110,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4093,9 +4149,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4144,10 +4200,10 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4215,12 +4271,12 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4296,7 +4352,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4336,9 +4392,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4409,7 +4465,7 @@
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4448,7 +4504,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -4496,11 +4552,11 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4567,12 +4623,12 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4639,9 +4695,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4677,11 +4733,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6844A23B-4865-4BC7-8285-CA3C17CB7B4E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4717,12 +4773,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+      <selection sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4771,10 +4827,10 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4821,6 +4877,175 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E739D59-5255-4A35-B887-CDB80DECF2C9}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="19.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E4" t="s">
+        <v>281</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BA4B24-2F40-43F0-9CFE-34A734E67A18}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4833,9 +5058,9 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4893,10 +5118,10 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4983,7 +5208,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5023,9 +5248,9 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Geards -add view edit search filter breadcrumbs
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3724A03F-4350-4E9F-B063-7D9D556904CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C03AA6-A52B-4D2D-8670-8AD0240AF18F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9240" windowHeight="5745" tabRatio="911" firstSheet="44" activeTab="51" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11820" windowHeight="7125" tabRatio="911" firstSheet="64" activeTab="71" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -80,6 +80,11 @@
     <sheet name="view_programs" sheetId="72" r:id="rId65"/>
     <sheet name="filter_programs" sheetId="74" r:id="rId66"/>
     <sheet name="edit_programs" sheetId="73" r:id="rId67"/>
+    <sheet name="add_new_grades" sheetId="75" r:id="rId68"/>
+    <sheet name="search_grades" sheetId="77" r:id="rId69"/>
+    <sheet name="view_grades" sheetId="76" r:id="rId70"/>
+    <sheet name="filter_grades" sheetId="78" r:id="rId71"/>
+    <sheet name="edit_grades" sheetId="79" r:id="rId72"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -91,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="344">
   <si>
     <t>Y</t>
   </si>
@@ -1051,6 +1056,78 @@
   </si>
   <si>
     <t>bio</t>
+  </si>
+  <si>
+    <t>grade1</t>
+  </si>
+  <si>
+    <t>marksfrom1</t>
+  </si>
+  <si>
+    <t>marksto1</t>
+  </si>
+  <si>
+    <t>gradepoint1</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Auto_GR_001</t>
+  </si>
+  <si>
+    <t>Engineering Grades</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>Distinction</t>
+  </si>
+  <si>
+    <t>Auto_GR</t>
+  </si>
+  <si>
+    <t>_GR_</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Auto_UPD_GR_001</t>
+  </si>
+  <si>
+    <t>Updated Engineering Grades</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>new marksfrom1</t>
+  </si>
+  <si>
+    <t>new marksto1</t>
+  </si>
+  <si>
+    <t>new gradepoint1</t>
+  </si>
+  <si>
+    <t>new Interpretation</t>
+  </si>
+  <si>
+    <t>Very Good</t>
   </si>
 </sst>
 </file>
@@ -4693,7 +4770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923C27E3-C15F-465A-8C31-E4DAE8B30273}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -5406,7 +5483,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5522,7 +5599,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5556,7 +5633,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5595,7 +5672,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5654,7 +5731,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5730,6 +5807,115 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E001ECD6-38F4-450A-9488-E4197B0C5BBD}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="7" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FF26D7-F243-4551-AB1B-380D9A81D39B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
@@ -5820,6 +6006,165 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B771D15B-1101-4F25-9424-CA0FF4311939}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5770AF16-D417-40F0-AE08-5A306503B3CD}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC8A70C-1D7B-4803-B8D7-85353F75B6D7}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H1" t="s">
+        <v>342</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <sheetPr codeName="Sheet28"/>

</xml_diff>

<commit_message>
added data reading from excel. finished further steps in program definitions adding
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\SLIIT\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C6E6A5-7576-47D7-97B3-14560F01B798}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3970D301-D9AA-4A34-94FB-AD19D60EA11B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" firstSheet="59" activeTab="68" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" firstSheet="64" activeTab="72" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -80,8 +80,12 @@
     <sheet name="view_programs" sheetId="72" r:id="rId65"/>
     <sheet name="filter_programs" sheetId="74" r:id="rId66"/>
     <sheet name="edit_programs" sheetId="73" r:id="rId67"/>
-    <sheet name="filterSubjects" sheetId="75" r:id="rId68"/>
-    <sheet name="add_subjects" sheetId="76" r:id="rId69"/>
+    <sheet name="add_new_grades" sheetId="75" r:id="rId68"/>
+    <sheet name="search_grades" sheetId="77" r:id="rId69"/>
+    <sheet name="view_grades" sheetId="76" r:id="rId70"/>
+    <sheet name="filter_grades" sheetId="78" r:id="rId71"/>
+    <sheet name="edit_grades" sheetId="79" r:id="rId72"/>
+    <sheet name="createNewProgramDefinitions" sheetId="80" r:id="rId73"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="351">
   <si>
     <t>Y</t>
   </si>
@@ -1055,58 +1059,97 @@
     <t>bio</t>
   </si>
   <si>
-    <t>SUN03</t>
-  </si>
-  <si>
-    <t>Computer</t>
-  </si>
-  <si>
-    <t>credits</t>
-  </si>
-  <si>
-    <t>dept</t>
-  </si>
-  <si>
-    <t>sessioncode</t>
-  </si>
-  <si>
-    <t>sessionname</t>
+    <t>grade1</t>
+  </si>
+  <si>
+    <t>marksfrom1</t>
+  </si>
+  <si>
+    <t>marksto1</t>
+  </si>
+  <si>
+    <t>gradepoint1</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Auto_GR_001</t>
+  </si>
+  <si>
+    <t>Engineering Grades</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>Distinction</t>
+  </si>
+  <si>
+    <t>Auto_GR</t>
+  </si>
+  <si>
+    <t>_GR_</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Auto_UPD_GR_001</t>
+  </si>
+  <si>
+    <t>Updated Engineering Grades</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>new marksfrom1</t>
+  </si>
+  <si>
+    <t>new marksto1</t>
+  </si>
+  <si>
+    <t>new gradepoint1</t>
+  </si>
+  <si>
+    <t>new Interpretation</t>
+  </si>
+  <si>
+    <t>Very Good</t>
   </si>
   <si>
     <t>priority</t>
   </si>
   <si>
-    <t>Auto_SBJ_001</t>
-  </si>
-  <si>
-    <t>sub001</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>Auto_SBJ_002</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>sub002</t>
-  </si>
-  <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>Auto_SBJ_003</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>sub003</t>
-  </si>
-  <si>
-    <t>Third</t>
+    <t>passes</t>
+  </si>
+  <si>
+    <t>semester</t>
+  </si>
+  <si>
+    <t>pr-4</t>
+  </si>
+  <si>
+    <t>exterior desigining</t>
+  </si>
+  <si>
+    <t>sem1</t>
+  </si>
+  <si>
+    <t>2020</t>
   </si>
 </sst>
 </file>
@@ -5462,7 +5505,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05"/>
@@ -5578,7 +5621,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05"/>
@@ -5612,7 +5655,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05"/>
@@ -5651,7 +5694,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05"/>
@@ -5710,7 +5753,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05"/>
@@ -5787,171 +5830,111 @@
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA01C1A-EA57-4F5E-89F8-359AC2432B39}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E001ECD6-38F4-450A-9488-E4197B0C5BBD}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="6" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F963038C-01FA-46ED-A947-29D79417FB2A}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
-  <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="6" max="6" width="19.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E1" t="s">
         <v>322</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>323</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" t="s">
         <v>324</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>325</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="B2" t="s">
         <v>326</v>
       </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="C2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FF26D7-F243-4551-AB1B-380D9A81D39B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>327</v>
-      </c>
-      <c r="B2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" t="s">
-        <v>328</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>330</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E3" t="s">
-        <v>332</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>334</v>
-      </c>
-      <c r="B4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="E4" t="s">
-        <v>336</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6045,6 +6028,230 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B771D15B-1101-4F25-9424-CA0FF4311939}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5770AF16-D417-40F0-AE08-5A306503B3CD}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC8A70C-1D7B-4803-B8D7-85353F75B6D7}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05"/>
+  <cols>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H1" t="s">
+        <v>342</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B2015A-E3A4-48C6-A9BA-28F340EC5718}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05"/>
+  <cols>
+    <col min="3" max="5" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="F2" t="s">
+        <v>349</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <sheetPr codeName="Sheet28"/>

</xml_diff>

<commit_message>
added updated excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Downloads\Microsoft.SkypeApp_kzf8qxf38zg5c!App\All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C03AA6-A52B-4D2D-8670-8AD0240AF18F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ABBCBE-F2EF-4885-9057-B77DFA85F500}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11820" windowHeight="7125" tabRatio="911" firstSheet="64" activeTab="71" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" firstSheet="64" activeTab="72" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -85,6 +85,7 @@
     <sheet name="view_grades" sheetId="76" r:id="rId70"/>
     <sheet name="filter_grades" sheetId="78" r:id="rId71"/>
     <sheet name="edit_grades" sheetId="79" r:id="rId72"/>
+    <sheet name="createNewProgramDefinitions" sheetId="80" r:id="rId73"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="351">
   <si>
     <t>Y</t>
   </si>
@@ -1128,6 +1129,27 @@
   </si>
   <si>
     <t>Very Good</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>passes</t>
+  </si>
+  <si>
+    <t>semester</t>
+  </si>
+  <si>
+    <t>pr-4</t>
+  </si>
+  <si>
+    <t>exterior desigining</t>
+  </si>
+  <si>
+    <t>sem1</t>
+  </si>
+  <si>
+    <t>2020</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1506,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1617,9 +1639,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1702,9 +1724,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1762,10 +1784,10 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1852,10 +1874,10 @@
       <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1973,9 +1995,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2036,11 +2058,11 @@
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2160,9 +2182,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2220,7 +2242,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2276,9 +2298,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2365,9 +2387,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2429,9 +2451,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2493,13 +2515,13 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="5" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2603,7 +2625,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2635,11 +2657,11 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="5" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="5" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2696,7 +2718,7 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2735,10 +2757,10 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2822,10 +2844,10 @@
       <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2898,7 +2920,7 @@
       <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2930,7 +2952,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2962,10 +2984,10 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3009,9 +3031,9 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3073,11 +3095,11 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="6" width="25.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.88671875" customWidth="1"/>
+    <col min="5" max="6" width="25.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3220,7 +3242,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3268,7 +3290,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
@@ -3303,7 +3325,7 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3359,10 +3381,10 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
     <col min="4" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3392,7 +3414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="30">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="30.15">
       <c r="A2" s="7" t="s">
         <v>178</v>
       </c>
@@ -3412,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="30">
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="30.15">
       <c r="A3" s="7" t="s">
         <v>180</v>
       </c>
@@ -3445,7 +3467,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3500,7 +3522,7 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -3531,10 +3553,10 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3593,9 +3615,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3655,10 +3677,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3753,11 +3775,11 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3852,11 +3874,11 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3991,7 +4013,7 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4030,9 +4052,9 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4114,7 +4136,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
@@ -4164,12 +4186,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4245,7 +4267,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4292,7 +4314,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4331,9 +4353,9 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4382,10 +4404,10 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4453,16 +4475,16 @@
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" style="9" customWidth="1"/>
-    <col min="12" max="13" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="9" customWidth="1"/>
+    <col min="12" max="13" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4574,7 +4596,7 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4614,9 +4636,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4687,7 +4709,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4726,7 +4748,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -4774,12 +4796,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4883,12 +4905,12 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4964,7 +4986,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5003,7 +5025,7 @@
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5042,7 +5064,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -5090,11 +5112,11 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5161,12 +5183,12 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5233,9 +5255,9 @@
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5276,9 +5298,9 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5335,7 +5357,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5374,9 +5396,9 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -5425,10 +5447,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5486,11 +5508,11 @@
       <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="8" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="8" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5602,9 +5624,9 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5636,7 +5658,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5675,7 +5697,7 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -5734,14 +5756,14 @@
       <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5815,11 +5837,11 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="6" max="7" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="6" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5893,7 +5915,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5925,10 +5947,10 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6014,7 +6036,7 @@
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -6045,7 +6067,7 @@
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -6089,17 +6111,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC8A70C-1D7B-4803-B8D7-85353F75B6D7}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6162,6 +6184,71 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B2015A-E3A4-48C6-A9BA-28F340EC5718}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05"/>
+  <cols>
+    <col min="3" max="5" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="F2" t="s">
+        <v>349</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6174,7 +6261,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -6214,9 +6301,9 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
prog def - E,V,F,S,B and Save Draft
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\SLIIT\SLIIT\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3970D301-D9AA-4A34-94FB-AD19D60EA11B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF56FC76-B76B-4A2B-BF33-80C62014D776}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" firstSheet="64" activeTab="72" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10950" tabRatio="911" firstSheet="71" activeTab="76" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -86,6 +86,11 @@
     <sheet name="filter_grades" sheetId="78" r:id="rId71"/>
     <sheet name="edit_grades" sheetId="79" r:id="rId72"/>
     <sheet name="createNewProgramDefinitions" sheetId="80" r:id="rId73"/>
+    <sheet name="searchProgramDefinitions" sheetId="81" r:id="rId74"/>
+    <sheet name="view_ProgramDefinitions" sheetId="82" r:id="rId75"/>
+    <sheet name="filter_ProgramDefinitions" sheetId="84" r:id="rId76"/>
+    <sheet name="edit_ProgramDefinitions" sheetId="85" r:id="rId77"/>
+    <sheet name="saveDraft_ProgramDefinitions" sheetId="83" r:id="rId78"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -97,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="366">
   <si>
     <t>Y</t>
   </si>
@@ -1140,16 +1145,61 @@
     <t>semester</t>
   </si>
   <si>
-    <t>pr-4</t>
-  </si>
-  <si>
-    <t>exterior desigining</t>
-  </si>
-  <si>
-    <t>sem1</t>
-  </si>
-  <si>
-    <t>2020</t>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>semester1</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>_PR_</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Sheffield Hallam University</t>
+  </si>
+  <si>
+    <t>In-progress</t>
+  </si>
+  <si>
+    <t>Computer Science Engineering</t>
+  </si>
+  <si>
+    <t>Auto_UPD_PR_001</t>
+  </si>
+  <si>
+    <t>Updated Survey Program</t>
+  </si>
+  <si>
+    <t>AUTO_PR_001</t>
+  </si>
+  <si>
+    <t>Exterior Desigining</t>
+  </si>
+  <si>
+    <t>AUTO_PR_6</t>
+  </si>
+  <si>
+    <t>semester 1</t>
+  </si>
+  <si>
+    <t>new priority</t>
+  </si>
+  <si>
+    <t>new passes</t>
+  </si>
+  <si>
+    <t>new semester</t>
+  </si>
+  <si>
+    <t>semester 3</t>
   </si>
 </sst>
 </file>
@@ -1506,7 +1556,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1639,9 +1689,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1724,9 +1774,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1784,10 +1834,10 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1874,10 +1924,10 @@
       <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1995,9 +2045,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2058,11 +2108,11 @@
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2182,9 +2232,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2242,7 +2292,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2298,9 +2348,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2387,9 +2437,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2451,9 +2501,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2515,13 +2565,13 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="7" width="13.88671875" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2625,7 +2675,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2657,11 +2707,11 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="5" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="5" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2718,7 +2768,7 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2757,10 +2807,10 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2844,10 +2894,10 @@
       <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2920,7 +2970,7 @@
       <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2952,7 +3002,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2984,10 +3034,10 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3031,9 +3081,9 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3095,11 +3145,11 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="45.88671875" customWidth="1"/>
-    <col min="5" max="6" width="25.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="6" width="25.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3242,7 +3292,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3290,7 +3340,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
@@ -3325,7 +3375,7 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3381,10 +3431,10 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="42.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3414,7 +3464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="30.15">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A2" s="7" t="s">
         <v>178</v>
       </c>
@@ -3434,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="30.15">
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A3" s="7" t="s">
         <v>180</v>
       </c>
@@ -3467,7 +3517,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3522,7 +3572,7 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -3553,10 +3603,10 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3615,9 +3665,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3677,10 +3727,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3775,11 +3825,11 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3874,11 +3924,11 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4013,7 +4063,7 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4052,9 +4102,9 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4136,7 +4186,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
@@ -4186,12 +4236,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4267,7 +4317,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4314,7 +4364,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4353,9 +4403,9 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4404,10 +4454,10 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4475,16 +4525,16 @@
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="9" customWidth="1"/>
-    <col min="12" max="13" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="9" customWidth="1"/>
+    <col min="12" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4596,7 +4646,7 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4636,9 +4686,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4709,7 +4759,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4748,7 +4798,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -4796,12 +4846,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4905,12 +4955,12 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4986,7 +5036,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5025,7 +5075,7 @@
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5064,7 +5114,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -5112,11 +5162,11 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5183,12 +5233,12 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5255,9 +5305,9 @@
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5298,9 +5348,9 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5357,7 +5407,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5396,9 +5446,9 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -5447,10 +5497,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5508,11 +5558,11 @@
       <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="8" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5624,9 +5674,9 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5658,7 +5708,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5697,7 +5747,7 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -5756,14 +5806,14 @@
       <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5837,11 +5887,11 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="7" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5912,10 +5962,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5947,10 +5997,10 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6030,13 +6080,13 @@
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B771D15B-1101-4F25-9424-CA0FF4311939}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -6054,6 +6104,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6064,10 +6122,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -6112,16 +6170,16 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+      <selection activeCell="I2" sqref="A1:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6191,13 +6249,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B2015A-E3A4-48C6-A9BA-28F340EC5718}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="5" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="5" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -6225,30 +6285,337 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0788559B-4A0E-486B-893E-D24BC3D81107}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790FAC59-D21F-473C-8016-B7F224C98D79}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33686EE1-951B-4522-B65B-5ACC62852ED2}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
         <v>347</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>353</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFA886C-6596-44DA-BB7A-942ADD19094A}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" t="s">
+        <v>364</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>365</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22D8DE-2A37-4182-8A1F-47077775AECD}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
         <v>348</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F2" t="s">
-        <v>349</v>
-      </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6261,7 +6628,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -6301,9 +6668,9 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Program definition Bug fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF56FC76-B76B-4A2B-BF33-80C62014D776}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840E73E4-B5A0-4635-B3B9-E2FD7D510F71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10950" tabRatio="911" firstSheet="71" activeTab="76" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10950" tabRatio="911" firstSheet="69" activeTab="75" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -197,9 +197,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>library</t>
-  </si>
-  <si>
     <t>row</t>
   </si>
   <si>
@@ -515,9 +512,6 @@
     <t>Computing</t>
   </si>
   <si>
-    <t>cent</t>
-  </si>
-  <si>
     <t>Auto_DT_</t>
   </si>
   <si>
@@ -914,9 +908,6 @@
     <t>subject2</t>
   </si>
   <si>
-    <t>Combined maths</t>
-  </si>
-  <si>
     <t xml:space="preserve">A </t>
   </si>
   <si>
@@ -938,12 +929,6 @@
     <t>Sri Lankan</t>
   </si>
   <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>maths</t>
-  </si>
-  <si>
     <t>Graduate</t>
   </si>
   <si>
@@ -1200,6 +1185,21 @@
   </si>
   <si>
     <t>semester 3</t>
+  </si>
+  <si>
+    <t>Physical Science stream</t>
+  </si>
+  <si>
+    <t>Physical Science</t>
+  </si>
+  <si>
+    <t>london a/l</t>
+  </si>
+  <si>
+    <t>CEN</t>
+  </si>
+  <si>
+    <t>Auto_PR</t>
   </si>
 </sst>
 </file>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -1644,10 +1644,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1658,10 +1658,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -1696,10 +1696,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1707,10 +1707,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>134</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1718,10 +1718,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1729,10 +1729,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -1740,10 +1740,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -1781,7 +1781,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1842,13 +1842,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1856,13 +1856,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1870,13 +1870,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -1884,13 +1884,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1898,13 +1898,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -1938,7 +1938,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1949,10 +1949,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" t="s">
-        <v>106</v>
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -1963,10 +1963,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -1977,10 +1977,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -1991,10 +1991,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -2005,10 +2005,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -2019,10 +2019,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -2052,10 +2052,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>105</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2074,10 +2074,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -2123,7 +2123,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" t="s">
-        <v>91</v>
+        <v>164</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2151,13 +2151,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -2168,13 +2168,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -2185,13 +2185,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -2202,13 +2202,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -2239,7 +2239,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2296,7 +2296,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2304,34 +2304,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2355,13 +2355,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2369,13 +2369,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -2383,13 +2383,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -2397,13 +2397,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -2411,13 +2411,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -2444,10 +2444,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2455,10 +2455,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>135</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2466,10 +2466,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2477,7 +2477,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -2508,10 +2508,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2519,7 +2519,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -2530,10 +2530,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -2582,19 +2582,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
         <v>16</v>
@@ -2605,13 +2605,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" t="s">
         <v>123</v>
       </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -2620,10 +2620,10 @@
         <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
@@ -2634,13 +2634,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
         <v>147</v>
-      </c>
-      <c r="B3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" t="s">
-        <v>149</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -2649,10 +2649,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -2679,7 +2679,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2716,19 +2716,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -2736,19 +2736,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -2772,7 +2772,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2815,10 +2815,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2826,10 +2826,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2837,10 +2837,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2848,10 +2848,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2859,10 +2859,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -2916,10 +2916,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" t="s">
-        <v>130</v>
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -2930,10 +2930,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2944,10 +2944,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -2974,7 +2974,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3006,7 +3006,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3014,10 +3014,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3042,13 +3042,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3056,13 +3056,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3088,10 +3088,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3099,10 +3099,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>138</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -3110,10 +3110,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -3121,7 +3121,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -3169,7 +3169,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -3183,16 +3183,16 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -3212,10 +3212,10 @@
         <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
@@ -3235,10 +3235,10 @@
         <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -3258,10 +3258,10 @@
         <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
@@ -3296,7 +3296,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3347,7 +3347,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3355,7 +3355,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3379,7 +3379,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3428,7 +3428,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3440,22 +3440,22 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
         <v>175</v>
       </c>
-      <c r="B1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>177</v>
-      </c>
       <c r="E1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G1" t="s">
         <v>16</v>
@@ -3466,16 +3466,16 @@
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A2" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -3486,13 +3486,13 @@
     </row>
     <row r="3" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A3" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>7</v>
@@ -3521,7 +3521,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -3545,7 +3545,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -3553,7 +3553,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -3576,7 +3576,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3584,7 +3584,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -3611,13 +3611,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3625,13 +3625,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -3639,13 +3639,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -3672,10 +3672,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3683,10 +3683,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -3694,10 +3694,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -3705,10 +3705,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -3742,19 +3742,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" t="s">
         <v>199</v>
       </c>
-      <c r="F1" t="s">
-        <v>201</v>
-      </c>
       <c r="G1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -3762,13 +3762,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2" t="s">
         <v>194</v>
       </c>
+      <c r="B2" t="s">
+        <v>192</v>
+      </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -3788,13 +3788,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -3834,25 +3834,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" t="s">
         <v>199</v>
       </c>
-      <c r="F1" t="s">
-        <v>201</v>
-      </c>
       <c r="G1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -3860,16 +3860,16 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" t="s">
         <v>202</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>204</v>
-      </c>
-      <c r="D2" t="s">
-        <v>206</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -3886,16 +3886,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" t="s">
         <v>203</v>
       </c>
-      <c r="C3" t="s">
-        <v>205</v>
-      </c>
       <c r="D3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -3950,13 +3950,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>232</v>
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>230</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -3967,13 +3967,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -3984,10 +3984,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -4001,13 +4001,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -4018,10 +4018,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -4035,10 +4035,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -4067,7 +4067,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4075,7 +4075,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4083,7 +4083,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4109,10 +4109,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -4120,10 +4120,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>207</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>205</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -4131,10 +4131,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -4142,10 +4142,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -4153,10 +4153,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -4164,10 +4164,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -4193,7 +4193,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4201,7 +4201,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4217,7 +4217,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -4252,10 +4252,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -4266,16 +4266,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" t="s">
-        <v>215</v>
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -4286,16 +4286,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -4321,7 +4321,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4345,7 +4345,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -4368,7 +4368,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4376,7 +4376,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4384,7 +4384,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4410,10 +4410,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -4421,10 +4421,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>264</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>262</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -4432,10 +4432,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -4463,16 +4463,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -4480,16 +4480,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>214</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>212</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -4497,16 +4497,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -4522,7 +4522,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4548,22 +4548,22 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G1" t="s">
         <v>267</v>
       </c>
-      <c r="F1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G1" t="s">
-        <v>269</v>
-      </c>
       <c r="H1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="I1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -4571,28 +4571,28 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B2" t="s">
-        <v>272</v>
+        <v>270</v>
+      </c>
+      <c r="B2" t="s">
+        <v>269</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E2" t="s">
-        <v>279</v>
+        <v>361</v>
       </c>
       <c r="F2" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="G2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -4603,28 +4603,28 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>278</v>
+        <v>363</v>
       </c>
       <c r="E3" t="s">
-        <v>279</v>
+        <v>362</v>
       </c>
       <c r="F3" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="G3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I3">
         <v>5</v>
@@ -4650,7 +4650,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4658,7 +4658,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4666,7 +4666,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4693,10 +4693,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -4704,10 +4704,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>114</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -4715,10 +4715,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -4726,7 +4726,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -4737,7 +4737,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -4763,7 +4763,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -4771,7 +4771,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4779,7 +4779,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4802,10 +4802,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -4813,10 +4813,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>284</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>279</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -4824,10 +4824,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -4857,28 +4857,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="G1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="H1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -4886,25 +4886,25 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>286</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>281</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E2" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H2">
         <v>4</v>
@@ -4915,25 +4915,25 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -4971,10 +4971,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -4985,16 +4985,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" t="s">
         <v>242</v>
-      </c>
-      <c r="C2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D2" t="s">
-        <v>244</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -5005,16 +5005,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -5040,7 +5040,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -5048,7 +5048,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5056,7 +5056,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5079,7 +5079,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -5087,7 +5087,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5095,7 +5095,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5118,10 +5118,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -5129,10 +5129,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>265</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>263</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -5140,10 +5140,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -5171,16 +5171,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -5188,16 +5188,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" t="s">
         <v>246</v>
       </c>
-      <c r="C2" t="s">
-        <v>248</v>
-      </c>
       <c r="D2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -5205,16 +5205,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" t="s">
         <v>247</v>
       </c>
-      <c r="C3" t="s">
-        <v>249</v>
-      </c>
       <c r="D3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -5243,7 +5243,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -5260,13 +5260,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>261</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>259</v>
       </c>
       <c r="C2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -5277,13 +5277,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -5312,7 +5312,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5328,7 +5328,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5355,7 +5355,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -5363,7 +5363,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5371,7 +5371,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5379,7 +5379,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -5387,7 +5387,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -5411,7 +5411,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -5419,7 +5419,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5427,7 +5427,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5453,10 +5453,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -5464,10 +5464,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>266</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>264</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -5475,10 +5475,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -5505,13 +5505,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -5519,13 +5519,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>255</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5533,13 +5533,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -5573,22 +5573,22 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="G1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I1" t="s">
         <v>16</v>
@@ -5599,28 +5599,28 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" t="s">
-        <v>291</v>
+        <v>285</v>
+      </c>
+      <c r="B2" t="s">
+        <v>286</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I2" t="s">
         <v>19</v>
@@ -5631,28 +5631,28 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" t="s">
+        <v>296</v>
+      </c>
+      <c r="E3" t="s">
+        <v>293</v>
+      </c>
+      <c r="F3" t="s">
         <v>291</v>
       </c>
-      <c r="C3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D3" t="s">
-        <v>301</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>289</v>
+      </c>
+      <c r="H3" t="s">
         <v>298</v>
-      </c>
-      <c r="F3" t="s">
-        <v>296</v>
-      </c>
-      <c r="G3" t="s">
-        <v>294</v>
-      </c>
-      <c r="H3" t="s">
-        <v>303</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
@@ -5681,7 +5681,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -5689,7 +5689,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5712,7 +5712,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -5720,7 +5720,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5728,7 +5728,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5751,10 +5751,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -5762,10 +5762,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>312</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>307</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -5773,10 +5773,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -5784,7 +5784,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -5818,28 +5818,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -5847,28 +5847,28 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>304</v>
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>299</v>
       </c>
       <c r="C2" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
@@ -5902,22 +5902,22 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="G1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="H1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -5925,25 +5925,25 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="B2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
@@ -5969,7 +5969,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -5977,7 +5977,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -6005,13 +6005,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -6019,13 +6019,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -6033,13 +6033,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -6047,13 +6047,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -6061,13 +6061,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -6090,7 +6090,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -6098,7 +6098,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -6106,7 +6106,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -6129,10 +6129,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -6140,10 +6140,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>332</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>327</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -6151,10 +6151,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -6184,28 +6184,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H1" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -6213,28 +6213,28 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>334</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>329</v>
       </c>
       <c r="C2" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D2" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>0</v>
@@ -6268,16 +6268,16 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -6285,22 +6285,22 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B2" t="s">
-        <v>359</v>
+        <v>353</v>
+      </c>
+      <c r="B2" t="s">
+        <v>354</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -6317,14 +6317,14 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -6332,7 +6332,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>331</v>
+        <v>365</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -6358,10 +6358,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>349</v>
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>344</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -6369,10 +6369,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -6387,8 +6387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33686EE1-951B-4522-B65B-5ACC62852ED2}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6398,10 +6398,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -6409,10 +6409,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>351</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>346</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -6420,10 +6420,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -6431,10 +6431,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -6442,10 +6442,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -6453,10 +6453,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -6464,10 +6464,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -6483,8 +6483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDFA886C-6596-44DA-BB7A-942ADD19094A}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6499,25 +6499,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G1" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -6525,25 +6525,25 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>356</v>
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>351</v>
       </c>
       <c r="C2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
@@ -6576,16 +6576,16 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -6593,22 +6593,22 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B2" t="s">
-        <v>347</v>
+        <v>355</v>
+      </c>
+      <c r="B2" t="s">
+        <v>342</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -6625,14 +6625,14 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -6640,7 +6640,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>364</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -6648,7 +6648,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -6681,10 +6681,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -6695,16 +6695,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -6715,16 +6715,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -6735,16 +6735,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -6755,16 +6755,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
@@ -6775,16 +6775,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
program types - column number change
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Downloads\Microsoft.SkypeApp_kzf8qxf38zg5c!App\All\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayashanig\Documents\Projects\SLIIT\Automation\SLIIT\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ABBCBE-F2EF-4885-9057-B77DFA85F500}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3079E952-6B7C-4A55-ABC3-F4D72D61AC2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" firstSheet="64" activeTab="72" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10950" tabRatio="911" firstSheet="38" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="add_new_locations" sheetId="9" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="350">
   <si>
     <t>Y</t>
   </si>
@@ -723,12 +723,6 @@
     <t>PT_001</t>
   </si>
   <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>Not Required</t>
-  </si>
-  <si>
     <t>Auto_QT_001</t>
   </si>
   <si>
@@ -1150,6 +1144,9 @@
   </si>
   <si>
     <t>2020</t>
+  </si>
+  <si>
+    <t>Not</t>
   </si>
 </sst>
 </file>
@@ -1506,7 +1503,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1597,7 +1594,7 @@
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1611,7 +1608,7 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -1639,9 +1636,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1724,9 +1721,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1784,10 +1781,10 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1874,10 +1871,10 @@
       <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1995,9 +1992,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2058,11 +2055,11 @@
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2182,9 +2179,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2242,7 +2239,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2298,9 +2295,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2387,9 +2384,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2451,9 +2448,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2515,13 +2512,13 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="7" width="13.88671875" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2570,7 +2567,7 @@
         <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G2" t="s">
         <v>190</v>
@@ -2599,10 +2596,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -2625,7 +2622,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2657,11 +2654,11 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="5" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="5" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2718,7 +2715,7 @@
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2757,10 +2754,10 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2844,10 +2841,10 @@
       <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2920,7 +2917,7 @@
       <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -2952,7 +2949,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2984,10 +2981,10 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3031,9 +3028,9 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3095,11 +3092,11 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="45.88671875" customWidth="1"/>
-    <col min="5" max="6" width="25.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="6" width="25.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3242,7 +3239,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3290,7 +3287,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
@@ -3325,7 +3322,7 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3381,10 +3378,10 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="42.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3414,7 +3411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="30.15">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A2" s="7" t="s">
         <v>178</v>
       </c>
@@ -3434,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="30.15">
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A3" s="7" t="s">
         <v>180</v>
       </c>
@@ -3467,7 +3464,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -3522,7 +3519,7 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -3553,10 +3550,10 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3615,9 +3612,9 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3677,10 +3674,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3775,11 +3772,11 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3874,11 +3871,11 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3903,10 +3900,10 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -3920,10 +3917,10 @@
         <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -3937,7 +3934,7 @@
         <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -3954,10 +3951,10 @@
         <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -3971,7 +3968,7 @@
         <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -3988,7 +3985,7 @@
         <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -4013,7 +4010,7 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4048,13 +4045,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FCBFFB-22A6-4482-83BD-FC8630938E34}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4106,7 +4103,7 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>349</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -4117,7 +4114,7 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>349</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -4133,10 +4130,10 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
@@ -4186,12 +4183,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4202,10 +4199,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -4216,16 +4213,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" t="s">
-        <v>215</v>
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -4236,16 +4233,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -4267,7 +4264,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4279,7 +4276,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4295,7 +4292,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -4314,7 +4311,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4353,9 +4350,9 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4374,7 +4371,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -4385,7 +4382,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -4404,10 +4401,10 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4422,7 +4419,7 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -4433,13 +4430,13 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -4450,13 +4447,13 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -4475,16 +4472,16 @@
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="9" customWidth="1"/>
-    <col min="12" max="13" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="9" customWidth="1"/>
+    <col min="12" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4501,19 +4498,19 @@
         <v>145</v>
       </c>
       <c r="E1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G1" t="s">
         <v>267</v>
       </c>
-      <c r="F1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G1" t="s">
-        <v>269</v>
-      </c>
       <c r="H1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -4521,28 +4518,28 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B2" t="s">
-        <v>272</v>
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
+        <v>270</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" t="s">
         <v>277</v>
       </c>
-      <c r="E2" t="s">
-        <v>279</v>
-      </c>
       <c r="F2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I2">
         <v>5</v>
@@ -4553,28 +4550,28 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I3">
         <v>5</v>
@@ -4596,7 +4593,7 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4608,7 +4605,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4616,7 +4613,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -4636,9 +4633,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4709,7 +4706,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4748,7 +4745,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -4766,7 +4763,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -4777,7 +4774,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -4796,12 +4793,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4816,19 +4813,19 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G1" t="s">
         <v>315</v>
       </c>
-      <c r="F1" t="s">
-        <v>289</v>
-      </c>
-      <c r="G1" t="s">
-        <v>317</v>
-      </c>
       <c r="H1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -4839,22 +4836,22 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G2" t="s">
         <v>286</v>
-      </c>
-      <c r="C2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F2" t="s">
-        <v>224</v>
-      </c>
-      <c r="G2" t="s">
-        <v>288</v>
       </c>
       <c r="H2">
         <v>4</v>
@@ -4868,22 +4865,22 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" t="s">
         <v>285</v>
       </c>
-      <c r="C3" t="s">
-        <v>287</v>
-      </c>
       <c r="D3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H3">
         <v>4</v>
@@ -4905,12 +4902,12 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4921,10 +4918,10 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -4935,16 +4932,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" t="s">
         <v>242</v>
-      </c>
-      <c r="C2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D2" t="s">
-        <v>244</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -4955,16 +4952,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -4986,7 +4983,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4998,7 +4995,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5006,7 +5003,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5025,7 +5022,7 @@
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5064,7 +5061,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -5082,7 +5079,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -5093,7 +5090,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -5112,11 +5109,11 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5130,7 +5127,7 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -5141,13 +5138,13 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" t="s">
         <v>246</v>
       </c>
-      <c r="C2" t="s">
-        <v>248</v>
-      </c>
       <c r="D2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -5158,13 +5155,13 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" t="s">
         <v>247</v>
       </c>
-      <c r="C3" t="s">
-        <v>249</v>
-      </c>
       <c r="D3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -5183,12 +5180,12 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5213,10 +5210,10 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -5230,10 +5227,10 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -5255,9 +5252,9 @@
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5270,7 +5267,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5278,7 +5275,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -5298,9 +5295,9 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5357,7 +5354,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5396,9 +5393,9 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -5417,7 +5414,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -5428,7 +5425,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -5447,10 +5444,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5472,10 +5469,10 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5486,10 +5483,10 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -5508,11 +5505,11 @@
       <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="8" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5526,19 +5523,19 @@
         <v>177</v>
       </c>
       <c r="D1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" t="s">
         <v>292</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>293</v>
-      </c>
-      <c r="G1" t="s">
-        <v>294</v>
-      </c>
-      <c r="H1" t="s">
-        <v>295</v>
       </c>
       <c r="I1" t="s">
         <v>16</v>
@@ -5549,28 +5546,28 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" t="s">
-        <v>291</v>
+        <v>288</v>
+      </c>
+      <c r="B2" t="s">
+        <v>289</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I2" t="s">
         <v>19</v>
@@ -5581,28 +5578,28 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
         <v>184</v>
       </c>
       <c r="D3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F3" t="s">
+        <v>294</v>
+      </c>
+      <c r="G3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H3" t="s">
         <v>301</v>
-      </c>
-      <c r="E3" t="s">
-        <v>298</v>
-      </c>
-      <c r="F3" t="s">
-        <v>296</v>
-      </c>
-      <c r="G3" t="s">
-        <v>294</v>
-      </c>
-      <c r="H3" t="s">
-        <v>303</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
@@ -5624,9 +5621,9 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5639,7 +5636,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5658,7 +5655,7 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5697,7 +5694,7 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -5715,7 +5712,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -5726,7 +5723,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -5756,14 +5753,14 @@
       <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5777,19 +5774,19 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G1" t="s">
+        <v>307</v>
+      </c>
+      <c r="H1" t="s">
         <v>308</v>
-      </c>
-      <c r="E1" t="s">
-        <v>307</v>
-      </c>
-      <c r="F1" t="s">
-        <v>311</v>
-      </c>
-      <c r="G1" t="s">
-        <v>309</v>
-      </c>
-      <c r="H1" t="s">
-        <v>310</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -5800,25 +5797,25 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D2" t="s">
         <v>184</v>
       </c>
       <c r="E2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
@@ -5837,11 +5834,11 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="7" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5852,22 +5849,22 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E1" t="s">
         <v>320</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>321</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H1" t="s">
         <v>322</v>
-      </c>
-      <c r="F1" t="s">
-        <v>323</v>
-      </c>
-      <c r="G1" t="s">
-        <v>329</v>
-      </c>
-      <c r="H1" t="s">
-        <v>324</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -5875,16 +5872,16 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" t="s">
         <v>325</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>328</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>151</v>
@@ -5893,7 +5890,7 @@
         <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
@@ -5915,7 +5912,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5927,7 +5924,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -5947,10 +5944,10 @@
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6036,7 +6033,7 @@
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -6067,7 +6064,7 @@
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
@@ -6085,7 +6082,7 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -6096,7 +6093,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -6115,13 +6112,13 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6135,19 +6132,19 @@
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" t="s">
         <v>339</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>340</v>
-      </c>
-      <c r="G1" t="s">
-        <v>341</v>
-      </c>
-      <c r="H1" t="s">
-        <v>342</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -6158,25 +6155,25 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D2" t="s">
         <v>334</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>0</v>
@@ -6191,13 +6188,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B2015A-E3A4-48C6-A9BA-28F340EC5718}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="5" width="8.88671875" style="2"/>
+    <col min="3" max="5" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -6208,16 +6205,16 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>175</v>
       </c>
       <c r="F1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -6225,10 +6222,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B2" t="s">
-        <v>348</v>
+        <v>345</v>
+      </c>
+      <c r="B2" t="s">
+        <v>346</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -6237,10 +6234,10 @@
         <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -6261,7 +6258,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -6301,9 +6298,9 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>